<commit_message>
Oracle SQL Join Types
</commit_message>
<xml_diff>
--- a/11.Joining-Multiple-Tables/Joining-Multiple-Tables.xlsx
+++ b/11.Joining-Multiple-Tables/Joining-Multiple-Tables.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\oracle\11.Joining-Multiple-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC81289-F1AD-423C-9EBB-78B1D6754CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789F1B94-FB6C-416F-BFF3-89922EDB9B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29175" yWindow="615" windowWidth="24990" windowHeight="13005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29175" yWindow="615" windowWidth="24990" windowHeight="13005" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oracle SQL Join Types" sheetId="1" r:id="rId1"/>
+    <sheet name="Natural Join" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>oracle</t>
     <phoneticPr fontId="1"/>
@@ -72,6 +73,124 @@
   </si>
   <si>
     <t>11.Joining-Multiple-Tables</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.Natural+Join+(Code+Samples).sql</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>oracle\11.Joining-Multiple-Tables\1.Natural+Join+(Code+Samples).sql</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/************* The Complete Oracle SQL Bootcamp *************</t>
+  </si>
+  <si>
+    <t> * Author  : Oracle Master Training                         *</t>
+  </si>
+  <si>
+    <t> * Course  : The Complete Oracle SQL Bootcamp               *</t>
+  </si>
+  <si>
+    <t> * Lecture : Natural Join                                   *</t>
+  </si>
+  <si>
+    <t> ************************************************************/</t>
+  </si>
+  <si>
+    <t>DESC employees;</t>
+  </si>
+  <si>
+    <t>DESC departments;</t>
+  </si>
+  <si>
+    <t>SELECT * FROM employees;</t>
+  </si>
+  <si>
+    <t>SELECT * FROM departments;</t>
+  </si>
+  <si>
+    <t>SELECT * FROM employees NATURAL JOIN departments;</t>
+  </si>
+  <si>
+    <t>SELECT * FROM departments NATURAL JOIN employees;</t>
+  </si>
+  <si>
+    <t>SELECT first_name, last_name, department_name FROM departments NATURAL JOIN employees;</t>
+  </si>
+  <si>
+    <t>DESC employees;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Natural join these 2 tables based on the common columns that have the same name(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEPARTMENT_ID, MANAGER_ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>→</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>these columns have the same data type and column name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SELECT * FROM employees NATURAL JOIN departments;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SELECT first_name, last_name, department_name FROM departments NATURAL JOIN employees;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We can also write some </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>specific</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> columns in the SELECT statement</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -79,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +218,14 @@
       <color rgb="FFFF0000"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -202,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -213,6 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -268,6 +396,275 @@
         <a:xfrm>
           <a:off x="796925" y="4254500"/>
           <a:ext cx="10550167" cy="4918075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>296182</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>102337</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CD6D0D8-9A92-D60E-7C2C-4B273E9887D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="786493" y="4284436"/>
+          <a:ext cx="11922578" cy="5761547"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>18584</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADADC2E1-0EDD-5B5A-8B93-D9F5D92CDD5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="777875" y="14706599"/>
+          <a:ext cx="6575425" cy="5428785"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>370568</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>84314</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="図 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AB1923D-F92A-7BB9-C075-7FE56E94B09A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="811893" y="21433971"/>
+          <a:ext cx="11965214" cy="5024161"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>182470</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>355414</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>74488</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="図 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C23E97BC-02C9-A0E0-1CBC-EA36AB89E790}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="843617" y="26333824"/>
+          <a:ext cx="12076766" cy="8030665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142501</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>86472</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>425824</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>83346</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="図 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BDF7F93-61E8-49FC-D632-B3E0435E06F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="803648" y="25860001"/>
+          <a:ext cx="12183970" cy="669227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134471</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>86472</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>201706</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>104807</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="図 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD44504D-CDFD-4D7E-1AE2-B3BD65BE8C83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="795618" y="36169413"/>
+          <a:ext cx="6678706" cy="8534806"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -544,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -668,4 +1065,2079 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA294ABD-A085-4C69-AD85-C262472CE730}">
+  <dimension ref="B3:T200"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O170" sqref="O170"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="2:13">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="4"/>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="4"/>
+      <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="46" spans="2:12">
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="B47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="3"/>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="B48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="5"/>
+    </row>
+    <row r="49" spans="2:15">
+      <c r="B49" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="51" spans="2:15">
+      <c r="B51" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="5"/>
+    </row>
+    <row r="52" spans="2:15">
+      <c r="B52" s="4"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="5"/>
+    </row>
+    <row r="53" spans="2:15">
+      <c r="B53" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="5"/>
+    </row>
+    <row r="54" spans="2:15">
+      <c r="B54" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="5"/>
+    </row>
+    <row r="55" spans="2:15">
+      <c r="B55" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="2:15">
+      <c r="B56" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="5"/>
+    </row>
+    <row r="57" spans="2:15">
+      <c r="B57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="5"/>
+    </row>
+    <row r="58" spans="2:15">
+      <c r="B58" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="5"/>
+    </row>
+    <row r="59" spans="2:15">
+      <c r="B59" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="5"/>
+    </row>
+    <row r="60" spans="2:15">
+      <c r="B60" s="7"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="9"/>
+    </row>
+    <row r="63" spans="2:15">
+      <c r="B63" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="3"/>
+      <c r="N63" t="s">
+        <v>28</v>
+      </c>
+      <c r="O63" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="2:15">
+      <c r="B64" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="5"/>
+    </row>
+    <row r="65" spans="2:13">
+      <c r="B65" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="5"/>
+    </row>
+    <row r="66" spans="2:13">
+      <c r="B66" s="4"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="5"/>
+    </row>
+    <row r="67" spans="2:13">
+      <c r="B67" s="4"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="5"/>
+    </row>
+    <row r="68" spans="2:13">
+      <c r="B68" s="4"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+      <c r="M68" s="5"/>
+    </row>
+    <row r="69" spans="2:13">
+      <c r="B69" s="4"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="5"/>
+    </row>
+    <row r="70" spans="2:13">
+      <c r="B70" s="4"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="5"/>
+    </row>
+    <row r="71" spans="2:13">
+      <c r="B71" s="4"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+      <c r="M71" s="5"/>
+    </row>
+    <row r="72" spans="2:13">
+      <c r="B72" s="4"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="5"/>
+    </row>
+    <row r="73" spans="2:13">
+      <c r="B73" s="4"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
+      <c r="M73" s="5"/>
+    </row>
+    <row r="74" spans="2:13">
+      <c r="B74" s="4"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
+      <c r="K74" s="10"/>
+      <c r="L74" s="10"/>
+      <c r="M74" s="5"/>
+    </row>
+    <row r="75" spans="2:13">
+      <c r="B75" s="4"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="5"/>
+    </row>
+    <row r="76" spans="2:13">
+      <c r="B76" s="4"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="J76" s="10"/>
+      <c r="K76" s="10"/>
+      <c r="L76" s="10"/>
+      <c r="M76" s="5"/>
+    </row>
+    <row r="77" spans="2:13">
+      <c r="B77" s="4"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
+      <c r="K77" s="10"/>
+      <c r="L77" s="10"/>
+      <c r="M77" s="5"/>
+    </row>
+    <row r="78" spans="2:13">
+      <c r="B78" s="4"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="10"/>
+      <c r="K78" s="10"/>
+      <c r="L78" s="10"/>
+      <c r="M78" s="5"/>
+    </row>
+    <row r="79" spans="2:13">
+      <c r="B79" s="4"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+      <c r="J79" s="10"/>
+      <c r="K79" s="10"/>
+      <c r="L79" s="10"/>
+      <c r="M79" s="5"/>
+    </row>
+    <row r="80" spans="2:13">
+      <c r="B80" s="4"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
+      <c r="J80" s="10"/>
+      <c r="K80" s="10"/>
+      <c r="L80" s="10"/>
+      <c r="M80" s="5"/>
+    </row>
+    <row r="81" spans="2:13">
+      <c r="B81" s="4"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="10"/>
+      <c r="K81" s="10"/>
+      <c r="L81" s="10"/>
+      <c r="M81" s="5"/>
+    </row>
+    <row r="82" spans="2:13">
+      <c r="B82" s="4"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
+      <c r="J82" s="10"/>
+      <c r="K82" s="10"/>
+      <c r="L82" s="10"/>
+      <c r="M82" s="5"/>
+    </row>
+    <row r="83" spans="2:13">
+      <c r="B83" s="4"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10"/>
+      <c r="K83" s="10"/>
+      <c r="L83" s="10"/>
+      <c r="M83" s="5"/>
+    </row>
+    <row r="84" spans="2:13">
+      <c r="B84" s="4"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="10"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="5"/>
+    </row>
+    <row r="85" spans="2:13">
+      <c r="B85" s="4"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
+      <c r="I85" s="10"/>
+      <c r="J85" s="10"/>
+      <c r="K85" s="10"/>
+      <c r="L85" s="10"/>
+      <c r="M85" s="5"/>
+    </row>
+    <row r="86" spans="2:13">
+      <c r="B86" s="4"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="10"/>
+      <c r="J86" s="10"/>
+      <c r="K86" s="10"/>
+      <c r="L86" s="10"/>
+      <c r="M86" s="5"/>
+    </row>
+    <row r="87" spans="2:13">
+      <c r="B87" s="4"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+      <c r="J87" s="10"/>
+      <c r="K87" s="10"/>
+      <c r="L87" s="10"/>
+      <c r="M87" s="5"/>
+    </row>
+    <row r="88" spans="2:13">
+      <c r="B88" s="4"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+      <c r="J88" s="10"/>
+      <c r="K88" s="10"/>
+      <c r="L88" s="10"/>
+      <c r="M88" s="5"/>
+    </row>
+    <row r="89" spans="2:13">
+      <c r="B89" s="4"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="5"/>
+    </row>
+    <row r="90" spans="2:13">
+      <c r="B90" s="7"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="8"/>
+      <c r="K90" s="8"/>
+      <c r="L90" s="8"/>
+      <c r="M90" s="9"/>
+    </row>
+    <row r="121" spans="2:20">
+      <c r="B121" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+      <c r="L121" s="2"/>
+      <c r="M121" s="2"/>
+      <c r="N121" s="2"/>
+      <c r="O121" s="2"/>
+      <c r="P121" s="2"/>
+      <c r="Q121" s="2"/>
+      <c r="R121" s="2"/>
+      <c r="S121" s="2"/>
+      <c r="T121" s="3"/>
+    </row>
+    <row r="122" spans="2:20">
+      <c r="B122" s="4"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10"/>
+      <c r="I122" s="10"/>
+      <c r="J122" s="10"/>
+      <c r="K122" s="10"/>
+      <c r="L122" s="10"/>
+      <c r="M122" s="10"/>
+      <c r="N122" s="10"/>
+      <c r="O122" s="10"/>
+      <c r="P122" s="10"/>
+      <c r="Q122" s="10"/>
+      <c r="R122" s="10"/>
+      <c r="S122" s="10"/>
+      <c r="T122" s="5"/>
+    </row>
+    <row r="123" spans="2:20">
+      <c r="B123" s="4"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+      <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
+      <c r="J123" s="10"/>
+      <c r="K123" s="10"/>
+      <c r="L123" s="10"/>
+      <c r="M123" s="10"/>
+      <c r="N123" s="10"/>
+      <c r="O123" s="10"/>
+      <c r="P123" s="10"/>
+      <c r="Q123" s="10"/>
+      <c r="R123" s="10"/>
+      <c r="S123" s="10"/>
+      <c r="T123" s="5"/>
+    </row>
+    <row r="124" spans="2:20">
+      <c r="B124" s="4"/>
+      <c r="C124" s="10"/>
+      <c r="D124" s="10"/>
+      <c r="E124" s="10"/>
+      <c r="F124" s="10"/>
+      <c r="G124" s="10"/>
+      <c r="H124" s="10"/>
+      <c r="I124" s="10"/>
+      <c r="J124" s="10"/>
+      <c r="K124" s="10"/>
+      <c r="L124" s="10"/>
+      <c r="M124" s="10"/>
+      <c r="N124" s="10"/>
+      <c r="O124" s="10"/>
+      <c r="P124" s="10"/>
+      <c r="Q124" s="10"/>
+      <c r="R124" s="10"/>
+      <c r="S124" s="10"/>
+      <c r="T124" s="5"/>
+    </row>
+    <row r="125" spans="2:20">
+      <c r="B125" s="4"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
+      <c r="F125" s="10"/>
+      <c r="G125" s="10"/>
+      <c r="H125" s="10"/>
+      <c r="I125" s="10"/>
+      <c r="J125" s="10"/>
+      <c r="K125" s="10"/>
+      <c r="L125" s="10"/>
+      <c r="M125" s="10"/>
+      <c r="N125" s="10"/>
+      <c r="O125" s="10"/>
+      <c r="P125" s="10"/>
+      <c r="Q125" s="10"/>
+      <c r="R125" s="10"/>
+      <c r="S125" s="10"/>
+      <c r="T125" s="5"/>
+    </row>
+    <row r="126" spans="2:20">
+      <c r="B126" s="4"/>
+      <c r="C126" s="10"/>
+      <c r="D126" s="10"/>
+      <c r="E126" s="10"/>
+      <c r="F126" s="10"/>
+      <c r="G126" s="10"/>
+      <c r="H126" s="10"/>
+      <c r="I126" s="10"/>
+      <c r="J126" s="10"/>
+      <c r="K126" s="10"/>
+      <c r="L126" s="10"/>
+      <c r="M126" s="10"/>
+      <c r="N126" s="10"/>
+      <c r="O126" s="10"/>
+      <c r="P126" s="10"/>
+      <c r="Q126" s="10"/>
+      <c r="R126" s="10"/>
+      <c r="S126" s="10"/>
+      <c r="T126" s="5"/>
+    </row>
+    <row r="127" spans="2:20">
+      <c r="B127" s="4"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+      <c r="F127" s="10"/>
+      <c r="G127" s="10"/>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+      <c r="J127" s="10"/>
+      <c r="K127" s="10"/>
+      <c r="L127" s="10"/>
+      <c r="M127" s="10"/>
+      <c r="N127" s="10"/>
+      <c r="O127" s="10"/>
+      <c r="P127" s="10"/>
+      <c r="Q127" s="10"/>
+      <c r="R127" s="10"/>
+      <c r="S127" s="10"/>
+      <c r="T127" s="5"/>
+    </row>
+    <row r="128" spans="2:20">
+      <c r="B128" s="4"/>
+      <c r="C128" s="10"/>
+      <c r="D128" s="10"/>
+      <c r="E128" s="10"/>
+      <c r="F128" s="10"/>
+      <c r="G128" s="10"/>
+      <c r="H128" s="10"/>
+      <c r="I128" s="10"/>
+      <c r="J128" s="10"/>
+      <c r="K128" s="10"/>
+      <c r="L128" s="10"/>
+      <c r="M128" s="10"/>
+      <c r="N128" s="10"/>
+      <c r="O128" s="10"/>
+      <c r="P128" s="10"/>
+      <c r="Q128" s="10"/>
+      <c r="R128" s="10"/>
+      <c r="S128" s="10"/>
+      <c r="T128" s="5"/>
+    </row>
+    <row r="129" spans="2:20">
+      <c r="B129" s="4"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
+      <c r="F129" s="10"/>
+      <c r="G129" s="10"/>
+      <c r="H129" s="10"/>
+      <c r="I129" s="10"/>
+      <c r="J129" s="10"/>
+      <c r="K129" s="10"/>
+      <c r="L129" s="10"/>
+      <c r="M129" s="10"/>
+      <c r="N129" s="10"/>
+      <c r="O129" s="10"/>
+      <c r="P129" s="10"/>
+      <c r="Q129" s="10"/>
+      <c r="R129" s="10"/>
+      <c r="S129" s="10"/>
+      <c r="T129" s="5"/>
+    </row>
+    <row r="130" spans="2:20">
+      <c r="B130" s="4"/>
+      <c r="C130" s="10"/>
+      <c r="D130" s="10"/>
+      <c r="E130" s="10"/>
+      <c r="F130" s="10"/>
+      <c r="G130" s="10"/>
+      <c r="H130" s="10"/>
+      <c r="I130" s="10"/>
+      <c r="J130" s="10"/>
+      <c r="K130" s="10"/>
+      <c r="L130" s="10"/>
+      <c r="M130" s="10"/>
+      <c r="N130" s="10"/>
+      <c r="O130" s="10"/>
+      <c r="P130" s="10"/>
+      <c r="Q130" s="10"/>
+      <c r="R130" s="10"/>
+      <c r="S130" s="10"/>
+      <c r="T130" s="5"/>
+    </row>
+    <row r="131" spans="2:20">
+      <c r="B131" s="4"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10"/>
+      <c r="H131" s="10"/>
+      <c r="I131" s="10"/>
+      <c r="J131" s="10"/>
+      <c r="K131" s="10"/>
+      <c r="L131" s="10"/>
+      <c r="M131" s="10"/>
+      <c r="N131" s="10"/>
+      <c r="O131" s="10"/>
+      <c r="P131" s="10"/>
+      <c r="Q131" s="10"/>
+      <c r="R131" s="10"/>
+      <c r="S131" s="10"/>
+      <c r="T131" s="5"/>
+    </row>
+    <row r="132" spans="2:20">
+      <c r="B132" s="4"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
+      <c r="F132" s="10"/>
+      <c r="G132" s="10"/>
+      <c r="H132" s="10"/>
+      <c r="I132" s="10"/>
+      <c r="J132" s="10"/>
+      <c r="K132" s="10"/>
+      <c r="L132" s="10"/>
+      <c r="M132" s="10"/>
+      <c r="N132" s="10"/>
+      <c r="O132" s="10"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="10"/>
+      <c r="R132" s="10"/>
+      <c r="S132" s="10"/>
+      <c r="T132" s="5"/>
+    </row>
+    <row r="133" spans="2:20">
+      <c r="B133" s="4"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
+      <c r="F133" s="10"/>
+      <c r="G133" s="10"/>
+      <c r="H133" s="10"/>
+      <c r="I133" s="10"/>
+      <c r="J133" s="10"/>
+      <c r="K133" s="10"/>
+      <c r="L133" s="10"/>
+      <c r="M133" s="10"/>
+      <c r="N133" s="10"/>
+      <c r="O133" s="10"/>
+      <c r="P133" s="10"/>
+      <c r="Q133" s="10"/>
+      <c r="R133" s="10"/>
+      <c r="S133" s="10"/>
+      <c r="T133" s="5"/>
+    </row>
+    <row r="134" spans="2:20">
+      <c r="B134" s="4"/>
+      <c r="C134" s="10"/>
+      <c r="D134" s="10"/>
+      <c r="E134" s="10"/>
+      <c r="F134" s="10"/>
+      <c r="G134" s="10"/>
+      <c r="H134" s="10"/>
+      <c r="I134" s="10"/>
+      <c r="J134" s="10"/>
+      <c r="K134" s="10"/>
+      <c r="L134" s="10"/>
+      <c r="M134" s="10"/>
+      <c r="N134" s="10"/>
+      <c r="O134" s="10"/>
+      <c r="P134" s="10"/>
+      <c r="Q134" s="10"/>
+      <c r="R134" s="10"/>
+      <c r="S134" s="10"/>
+      <c r="T134" s="5"/>
+    </row>
+    <row r="135" spans="2:20">
+      <c r="B135" s="4"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
+      <c r="F135" s="10"/>
+      <c r="G135" s="10"/>
+      <c r="H135" s="10"/>
+      <c r="I135" s="10"/>
+      <c r="J135" s="10"/>
+      <c r="K135" s="10"/>
+      <c r="L135" s="10"/>
+      <c r="M135" s="10"/>
+      <c r="N135" s="10"/>
+      <c r="O135" s="10"/>
+      <c r="P135" s="10"/>
+      <c r="Q135" s="10"/>
+      <c r="R135" s="10"/>
+      <c r="S135" s="10"/>
+      <c r="T135" s="5"/>
+    </row>
+    <row r="136" spans="2:20">
+      <c r="B136" s="4"/>
+      <c r="C136" s="10"/>
+      <c r="D136" s="10"/>
+      <c r="E136" s="10"/>
+      <c r="F136" s="10"/>
+      <c r="G136" s="10"/>
+      <c r="H136" s="10"/>
+      <c r="I136" s="10"/>
+      <c r="J136" s="10"/>
+      <c r="K136" s="10"/>
+      <c r="L136" s="10"/>
+      <c r="M136" s="10"/>
+      <c r="N136" s="10"/>
+      <c r="O136" s="10"/>
+      <c r="P136" s="10"/>
+      <c r="Q136" s="10"/>
+      <c r="R136" s="10"/>
+      <c r="S136" s="10"/>
+      <c r="T136" s="5"/>
+    </row>
+    <row r="137" spans="2:20">
+      <c r="B137" s="4"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
+      <c r="H137" s="10"/>
+      <c r="I137" s="10"/>
+      <c r="J137" s="10"/>
+      <c r="K137" s="10"/>
+      <c r="L137" s="10"/>
+      <c r="M137" s="10"/>
+      <c r="N137" s="10"/>
+      <c r="O137" s="10"/>
+      <c r="P137" s="10"/>
+      <c r="Q137" s="10"/>
+      <c r="R137" s="10"/>
+      <c r="S137" s="10"/>
+      <c r="T137" s="5"/>
+    </row>
+    <row r="138" spans="2:20">
+      <c r="B138" s="4"/>
+      <c r="C138" s="10"/>
+      <c r="D138" s="10"/>
+      <c r="E138" s="10"/>
+      <c r="F138" s="10"/>
+      <c r="G138" s="10"/>
+      <c r="H138" s="10"/>
+      <c r="I138" s="10"/>
+      <c r="J138" s="10"/>
+      <c r="K138" s="10"/>
+      <c r="L138" s="10"/>
+      <c r="M138" s="10"/>
+      <c r="N138" s="10"/>
+      <c r="O138" s="10"/>
+      <c r="P138" s="10"/>
+      <c r="Q138" s="10"/>
+      <c r="R138" s="10"/>
+      <c r="S138" s="10"/>
+      <c r="T138" s="5"/>
+    </row>
+    <row r="139" spans="2:20">
+      <c r="B139" s="4"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
+      <c r="F139" s="10"/>
+      <c r="G139" s="10"/>
+      <c r="H139" s="10"/>
+      <c r="I139" s="10"/>
+      <c r="J139" s="10"/>
+      <c r="K139" s="10"/>
+      <c r="L139" s="10"/>
+      <c r="M139" s="10"/>
+      <c r="N139" s="10"/>
+      <c r="O139" s="10"/>
+      <c r="P139" s="10"/>
+      <c r="Q139" s="10"/>
+      <c r="R139" s="10"/>
+      <c r="S139" s="10"/>
+      <c r="T139" s="5"/>
+    </row>
+    <row r="140" spans="2:20">
+      <c r="B140" s="4"/>
+      <c r="C140" s="10"/>
+      <c r="D140" s="10"/>
+      <c r="E140" s="10"/>
+      <c r="F140" s="10"/>
+      <c r="G140" s="10"/>
+      <c r="H140" s="10"/>
+      <c r="I140" s="10"/>
+      <c r="J140" s="10"/>
+      <c r="K140" s="10"/>
+      <c r="L140" s="10"/>
+      <c r="M140" s="10"/>
+      <c r="N140" s="10"/>
+      <c r="O140" s="10"/>
+      <c r="P140" s="10"/>
+      <c r="Q140" s="10"/>
+      <c r="R140" s="10"/>
+      <c r="S140" s="10"/>
+      <c r="T140" s="5"/>
+    </row>
+    <row r="141" spans="2:20">
+      <c r="B141" s="4"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
+      <c r="H141" s="10"/>
+      <c r="I141" s="10"/>
+      <c r="J141" s="10"/>
+      <c r="K141" s="10"/>
+      <c r="L141" s="10"/>
+      <c r="M141" s="10"/>
+      <c r="N141" s="10"/>
+      <c r="O141" s="10"/>
+      <c r="P141" s="10"/>
+      <c r="Q141" s="10"/>
+      <c r="R141" s="10"/>
+      <c r="S141" s="10"/>
+      <c r="T141" s="5"/>
+    </row>
+    <row r="142" spans="2:20">
+      <c r="B142" s="4"/>
+      <c r="C142" s="10"/>
+      <c r="D142" s="10"/>
+      <c r="E142" s="10"/>
+      <c r="F142" s="10"/>
+      <c r="G142" s="10"/>
+      <c r="H142" s="10"/>
+      <c r="I142" s="10"/>
+      <c r="J142" s="10"/>
+      <c r="K142" s="10"/>
+      <c r="L142" s="10"/>
+      <c r="M142" s="10"/>
+      <c r="N142" s="10"/>
+      <c r="O142" s="10"/>
+      <c r="P142" s="10"/>
+      <c r="Q142" s="10"/>
+      <c r="R142" s="10"/>
+      <c r="S142" s="10"/>
+      <c r="T142" s="5"/>
+    </row>
+    <row r="143" spans="2:20">
+      <c r="B143" s="4"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+      <c r="G143" s="10"/>
+      <c r="H143" s="10"/>
+      <c r="I143" s="10"/>
+      <c r="J143" s="10"/>
+      <c r="K143" s="10"/>
+      <c r="L143" s="10"/>
+      <c r="M143" s="10"/>
+      <c r="N143" s="10"/>
+      <c r="O143" s="10"/>
+      <c r="P143" s="10"/>
+      <c r="Q143" s="10"/>
+      <c r="R143" s="10"/>
+      <c r="S143" s="10"/>
+      <c r="T143" s="5"/>
+    </row>
+    <row r="144" spans="2:20">
+      <c r="B144" s="4"/>
+      <c r="C144" s="10"/>
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
+      <c r="F144" s="10"/>
+      <c r="G144" s="10"/>
+      <c r="H144" s="10"/>
+      <c r="I144" s="10"/>
+      <c r="J144" s="10"/>
+      <c r="K144" s="10"/>
+      <c r="L144" s="10"/>
+      <c r="M144" s="10"/>
+      <c r="N144" s="10"/>
+      <c r="O144" s="10"/>
+      <c r="P144" s="10"/>
+      <c r="Q144" s="10"/>
+      <c r="R144" s="10"/>
+      <c r="S144" s="10"/>
+      <c r="T144" s="5"/>
+    </row>
+    <row r="145" spans="2:20">
+      <c r="B145" s="4"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
+      <c r="F145" s="10"/>
+      <c r="G145" s="10"/>
+      <c r="H145" s="10"/>
+      <c r="I145" s="10"/>
+      <c r="J145" s="10"/>
+      <c r="K145" s="10"/>
+      <c r="L145" s="10"/>
+      <c r="M145" s="10"/>
+      <c r="N145" s="10"/>
+      <c r="O145" s="10"/>
+      <c r="P145" s="10"/>
+      <c r="Q145" s="10"/>
+      <c r="R145" s="10"/>
+      <c r="S145" s="10"/>
+      <c r="T145" s="5"/>
+    </row>
+    <row r="146" spans="2:20">
+      <c r="B146" s="4"/>
+      <c r="C146" s="10"/>
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
+      <c r="F146" s="10"/>
+      <c r="G146" s="10"/>
+      <c r="H146" s="10"/>
+      <c r="I146" s="10"/>
+      <c r="J146" s="10"/>
+      <c r="K146" s="10"/>
+      <c r="L146" s="10"/>
+      <c r="M146" s="10"/>
+      <c r="N146" s="10"/>
+      <c r="O146" s="10"/>
+      <c r="P146" s="10"/>
+      <c r="Q146" s="10"/>
+      <c r="R146" s="10"/>
+      <c r="S146" s="10"/>
+      <c r="T146" s="5"/>
+    </row>
+    <row r="147" spans="2:20">
+      <c r="B147" s="4"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+      <c r="G147" s="10"/>
+      <c r="H147" s="10"/>
+      <c r="I147" s="10"/>
+      <c r="J147" s="10"/>
+      <c r="K147" s="10"/>
+      <c r="L147" s="10"/>
+      <c r="M147" s="10"/>
+      <c r="N147" s="10"/>
+      <c r="O147" s="10"/>
+      <c r="P147" s="10"/>
+      <c r="Q147" s="10"/>
+      <c r="R147" s="10"/>
+      <c r="S147" s="10"/>
+      <c r="T147" s="5"/>
+    </row>
+    <row r="148" spans="2:20">
+      <c r="B148" s="4"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="10"/>
+      <c r="F148" s="10"/>
+      <c r="G148" s="10"/>
+      <c r="H148" s="10"/>
+      <c r="I148" s="10"/>
+      <c r="J148" s="10"/>
+      <c r="K148" s="10"/>
+      <c r="L148" s="10"/>
+      <c r="M148" s="10"/>
+      <c r="N148" s="10"/>
+      <c r="O148" s="10"/>
+      <c r="P148" s="10"/>
+      <c r="Q148" s="10"/>
+      <c r="R148" s="10"/>
+      <c r="S148" s="10"/>
+      <c r="T148" s="5"/>
+    </row>
+    <row r="149" spans="2:20">
+      <c r="B149" s="4"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="10"/>
+      <c r="F149" s="10"/>
+      <c r="G149" s="10"/>
+      <c r="H149" s="10"/>
+      <c r="I149" s="10"/>
+      <c r="J149" s="10"/>
+      <c r="K149" s="10"/>
+      <c r="L149" s="10"/>
+      <c r="M149" s="10"/>
+      <c r="N149" s="10"/>
+      <c r="O149" s="10"/>
+      <c r="P149" s="10"/>
+      <c r="Q149" s="10"/>
+      <c r="R149" s="10"/>
+      <c r="S149" s="10"/>
+      <c r="T149" s="5"/>
+    </row>
+    <row r="150" spans="2:20">
+      <c r="B150" s="4"/>
+      <c r="C150" s="10"/>
+      <c r="D150" s="10"/>
+      <c r="E150" s="10"/>
+      <c r="F150" s="10"/>
+      <c r="G150" s="10"/>
+      <c r="H150" s="10"/>
+      <c r="I150" s="10"/>
+      <c r="J150" s="10"/>
+      <c r="K150" s="10"/>
+      <c r="L150" s="10"/>
+      <c r="M150" s="10"/>
+      <c r="N150" s="10"/>
+      <c r="O150" s="10"/>
+      <c r="P150" s="10"/>
+      <c r="Q150" s="10"/>
+      <c r="R150" s="10"/>
+      <c r="S150" s="10"/>
+      <c r="T150" s="5"/>
+    </row>
+    <row r="151" spans="2:20">
+      <c r="B151" s="4"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="10"/>
+      <c r="E151" s="10"/>
+      <c r="F151" s="10"/>
+      <c r="G151" s="10"/>
+      <c r="H151" s="10"/>
+      <c r="I151" s="10"/>
+      <c r="J151" s="10"/>
+      <c r="K151" s="10"/>
+      <c r="L151" s="10"/>
+      <c r="M151" s="10"/>
+      <c r="N151" s="10"/>
+      <c r="O151" s="10"/>
+      <c r="P151" s="10"/>
+      <c r="Q151" s="10"/>
+      <c r="R151" s="10"/>
+      <c r="S151" s="10"/>
+      <c r="T151" s="5"/>
+    </row>
+    <row r="152" spans="2:20">
+      <c r="B152" s="4"/>
+      <c r="C152" s="10"/>
+      <c r="D152" s="10"/>
+      <c r="E152" s="10"/>
+      <c r="F152" s="10"/>
+      <c r="G152" s="10"/>
+      <c r="H152" s="10"/>
+      <c r="I152" s="10"/>
+      <c r="J152" s="10"/>
+      <c r="K152" s="10"/>
+      <c r="L152" s="10"/>
+      <c r="M152" s="10"/>
+      <c r="N152" s="10"/>
+      <c r="O152" s="10"/>
+      <c r="P152" s="10"/>
+      <c r="Q152" s="10"/>
+      <c r="R152" s="10"/>
+      <c r="S152" s="10"/>
+      <c r="T152" s="5"/>
+    </row>
+    <row r="153" spans="2:20">
+      <c r="B153" s="4"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
+      <c r="E153" s="10"/>
+      <c r="F153" s="10"/>
+      <c r="G153" s="10"/>
+      <c r="H153" s="10"/>
+      <c r="I153" s="10"/>
+      <c r="J153" s="10"/>
+      <c r="K153" s="10"/>
+      <c r="L153" s="10"/>
+      <c r="M153" s="10"/>
+      <c r="N153" s="10"/>
+      <c r="O153" s="10"/>
+      <c r="P153" s="10"/>
+      <c r="Q153" s="10"/>
+      <c r="R153" s="10"/>
+      <c r="S153" s="10"/>
+      <c r="T153" s="5"/>
+    </row>
+    <row r="154" spans="2:20">
+      <c r="B154" s="4"/>
+      <c r="C154" s="10"/>
+      <c r="D154" s="10"/>
+      <c r="E154" s="10"/>
+      <c r="F154" s="10"/>
+      <c r="G154" s="10"/>
+      <c r="H154" s="10"/>
+      <c r="I154" s="10"/>
+      <c r="J154" s="10"/>
+      <c r="K154" s="10"/>
+      <c r="L154" s="10"/>
+      <c r="M154" s="10"/>
+      <c r="N154" s="10"/>
+      <c r="O154" s="10"/>
+      <c r="P154" s="10"/>
+      <c r="Q154" s="10"/>
+      <c r="R154" s="10"/>
+      <c r="S154" s="10"/>
+      <c r="T154" s="5"/>
+    </row>
+    <row r="155" spans="2:20">
+      <c r="B155" s="4"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
+      <c r="F155" s="10"/>
+      <c r="G155" s="10"/>
+      <c r="H155" s="10"/>
+      <c r="I155" s="10"/>
+      <c r="J155" s="10"/>
+      <c r="K155" s="10"/>
+      <c r="L155" s="10"/>
+      <c r="M155" s="10"/>
+      <c r="N155" s="10"/>
+      <c r="O155" s="10"/>
+      <c r="P155" s="10"/>
+      <c r="Q155" s="10"/>
+      <c r="R155" s="10"/>
+      <c r="S155" s="10"/>
+      <c r="T155" s="5"/>
+    </row>
+    <row r="156" spans="2:20">
+      <c r="B156" s="4"/>
+      <c r="C156" s="10"/>
+      <c r="D156" s="10"/>
+      <c r="E156" s="10"/>
+      <c r="F156" s="10"/>
+      <c r="G156" s="10"/>
+      <c r="H156" s="10"/>
+      <c r="I156" s="10"/>
+      <c r="J156" s="10"/>
+      <c r="K156" s="10"/>
+      <c r="L156" s="10"/>
+      <c r="M156" s="10"/>
+      <c r="N156" s="10"/>
+      <c r="O156" s="10"/>
+      <c r="P156" s="10"/>
+      <c r="Q156" s="10"/>
+      <c r="R156" s="10"/>
+      <c r="S156" s="10"/>
+      <c r="T156" s="5"/>
+    </row>
+    <row r="157" spans="2:20">
+      <c r="B157" s="4"/>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="10"/>
+      <c r="F157" s="10"/>
+      <c r="G157" s="10"/>
+      <c r="H157" s="10"/>
+      <c r="I157" s="10"/>
+      <c r="J157" s="10"/>
+      <c r="K157" s="10"/>
+      <c r="L157" s="10"/>
+      <c r="M157" s="10"/>
+      <c r="N157" s="10"/>
+      <c r="O157" s="10"/>
+      <c r="P157" s="10"/>
+      <c r="Q157" s="10"/>
+      <c r="R157" s="10"/>
+      <c r="S157" s="10"/>
+      <c r="T157" s="5"/>
+    </row>
+    <row r="158" spans="2:20">
+      <c r="B158" s="7"/>
+      <c r="C158" s="8"/>
+      <c r="D158" s="8"/>
+      <c r="E158" s="8"/>
+      <c r="F158" s="8"/>
+      <c r="G158" s="8"/>
+      <c r="H158" s="8"/>
+      <c r="I158" s="8"/>
+      <c r="J158" s="8"/>
+      <c r="K158" s="8"/>
+      <c r="L158" s="8"/>
+      <c r="M158" s="8"/>
+      <c r="N158" s="8"/>
+      <c r="O158" s="8"/>
+      <c r="P158" s="8"/>
+      <c r="Q158" s="8"/>
+      <c r="R158" s="8"/>
+      <c r="S158" s="8"/>
+      <c r="T158" s="9"/>
+    </row>
+    <row r="161" spans="2:14">
+      <c r="B161" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+      <c r="H161" s="2"/>
+      <c r="I161" s="2"/>
+      <c r="J161" s="2"/>
+      <c r="K161" s="2"/>
+      <c r="L161" s="3"/>
+      <c r="M161" t="s">
+        <v>28</v>
+      </c>
+      <c r="N161" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="162" spans="2:14">
+      <c r="B162" s="4"/>
+      <c r="C162" s="10"/>
+      <c r="D162" s="10"/>
+      <c r="E162" s="10"/>
+      <c r="F162" s="10"/>
+      <c r="G162" s="10"/>
+      <c r="H162" s="10"/>
+      <c r="I162" s="10"/>
+      <c r="J162" s="10"/>
+      <c r="K162" s="10"/>
+      <c r="L162" s="5"/>
+    </row>
+    <row r="163" spans="2:14">
+      <c r="B163" s="4"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
+      <c r="F163" s="10"/>
+      <c r="G163" s="10"/>
+      <c r="H163" s="10"/>
+      <c r="I163" s="10"/>
+      <c r="J163" s="10"/>
+      <c r="K163" s="10"/>
+      <c r="L163" s="5"/>
+    </row>
+    <row r="164" spans="2:14">
+      <c r="B164" s="4"/>
+      <c r="C164" s="10"/>
+      <c r="D164" s="10"/>
+      <c r="E164" s="10"/>
+      <c r="F164" s="10"/>
+      <c r="G164" s="10"/>
+      <c r="H164" s="10"/>
+      <c r="I164" s="10"/>
+      <c r="J164" s="10"/>
+      <c r="K164" s="10"/>
+      <c r="L164" s="5"/>
+    </row>
+    <row r="165" spans="2:14">
+      <c r="B165" s="4"/>
+      <c r="C165" s="10"/>
+      <c r="D165" s="10"/>
+      <c r="E165" s="10"/>
+      <c r="F165" s="10"/>
+      <c r="G165" s="10"/>
+      <c r="H165" s="10"/>
+      <c r="I165" s="10"/>
+      <c r="J165" s="10"/>
+      <c r="K165" s="10"/>
+      <c r="L165" s="5"/>
+    </row>
+    <row r="166" spans="2:14">
+      <c r="B166" s="4"/>
+      <c r="C166" s="10"/>
+      <c r="D166" s="10"/>
+      <c r="E166" s="10"/>
+      <c r="F166" s="10"/>
+      <c r="G166" s="10"/>
+      <c r="H166" s="10"/>
+      <c r="I166" s="10"/>
+      <c r="J166" s="10"/>
+      <c r="K166" s="10"/>
+      <c r="L166" s="5"/>
+    </row>
+    <row r="167" spans="2:14">
+      <c r="B167" s="4"/>
+      <c r="C167" s="10"/>
+      <c r="D167" s="10"/>
+      <c r="E167" s="10"/>
+      <c r="F167" s="10"/>
+      <c r="G167" s="10"/>
+      <c r="H167" s="10"/>
+      <c r="I167" s="10"/>
+      <c r="J167" s="10"/>
+      <c r="K167" s="10"/>
+      <c r="L167" s="5"/>
+    </row>
+    <row r="168" spans="2:14">
+      <c r="B168" s="4"/>
+      <c r="C168" s="10"/>
+      <c r="D168" s="10"/>
+      <c r="E168" s="10"/>
+      <c r="F168" s="10"/>
+      <c r="G168" s="10"/>
+      <c r="H168" s="10"/>
+      <c r="I168" s="10"/>
+      <c r="J168" s="10"/>
+      <c r="K168" s="10"/>
+      <c r="L168" s="5"/>
+    </row>
+    <row r="169" spans="2:14">
+      <c r="B169" s="4"/>
+      <c r="C169" s="10"/>
+      <c r="D169" s="10"/>
+      <c r="E169" s="10"/>
+      <c r="F169" s="10"/>
+      <c r="G169" s="10"/>
+      <c r="H169" s="10"/>
+      <c r="I169" s="10"/>
+      <c r="J169" s="10"/>
+      <c r="K169" s="10"/>
+      <c r="L169" s="5"/>
+    </row>
+    <row r="170" spans="2:14">
+      <c r="B170" s="4"/>
+      <c r="C170" s="10"/>
+      <c r="D170" s="10"/>
+      <c r="E170" s="10"/>
+      <c r="F170" s="10"/>
+      <c r="G170" s="10"/>
+      <c r="H170" s="10"/>
+      <c r="I170" s="10"/>
+      <c r="J170" s="10"/>
+      <c r="K170" s="10"/>
+      <c r="L170" s="5"/>
+    </row>
+    <row r="171" spans="2:14">
+      <c r="B171" s="4"/>
+      <c r="C171" s="10"/>
+      <c r="D171" s="10"/>
+      <c r="E171" s="10"/>
+      <c r="F171" s="10"/>
+      <c r="G171" s="10"/>
+      <c r="H171" s="10"/>
+      <c r="I171" s="10"/>
+      <c r="J171" s="10"/>
+      <c r="K171" s="10"/>
+      <c r="L171" s="5"/>
+    </row>
+    <row r="172" spans="2:14">
+      <c r="B172" s="4"/>
+      <c r="C172" s="10"/>
+      <c r="D172" s="10"/>
+      <c r="E172" s="10"/>
+      <c r="F172" s="10"/>
+      <c r="G172" s="10"/>
+      <c r="H172" s="10"/>
+      <c r="I172" s="10"/>
+      <c r="J172" s="10"/>
+      <c r="K172" s="10"/>
+      <c r="L172" s="5"/>
+    </row>
+    <row r="173" spans="2:14">
+      <c r="B173" s="4"/>
+      <c r="C173" s="10"/>
+      <c r="D173" s="10"/>
+      <c r="E173" s="10"/>
+      <c r="F173" s="10"/>
+      <c r="G173" s="10"/>
+      <c r="H173" s="10"/>
+      <c r="I173" s="10"/>
+      <c r="J173" s="10"/>
+      <c r="K173" s="10"/>
+      <c r="L173" s="5"/>
+    </row>
+    <row r="174" spans="2:14">
+      <c r="B174" s="4"/>
+      <c r="C174" s="10"/>
+      <c r="D174" s="10"/>
+      <c r="E174" s="10"/>
+      <c r="F174" s="10"/>
+      <c r="G174" s="10"/>
+      <c r="H174" s="10"/>
+      <c r="I174" s="10"/>
+      <c r="J174" s="10"/>
+      <c r="K174" s="10"/>
+      <c r="L174" s="5"/>
+    </row>
+    <row r="175" spans="2:14">
+      <c r="B175" s="4"/>
+      <c r="C175" s="10"/>
+      <c r="D175" s="10"/>
+      <c r="E175" s="10"/>
+      <c r="F175" s="10"/>
+      <c r="G175" s="10"/>
+      <c r="H175" s="10"/>
+      <c r="I175" s="10"/>
+      <c r="J175" s="10"/>
+      <c r="K175" s="10"/>
+      <c r="L175" s="5"/>
+    </row>
+    <row r="176" spans="2:14">
+      <c r="B176" s="4"/>
+      <c r="C176" s="10"/>
+      <c r="D176" s="10"/>
+      <c r="E176" s="10"/>
+      <c r="F176" s="10"/>
+      <c r="G176" s="10"/>
+      <c r="H176" s="10"/>
+      <c r="I176" s="10"/>
+      <c r="J176" s="10"/>
+      <c r="K176" s="10"/>
+      <c r="L176" s="5"/>
+    </row>
+    <row r="177" spans="2:12">
+      <c r="B177" s="4"/>
+      <c r="C177" s="10"/>
+      <c r="D177" s="10"/>
+      <c r="E177" s="10"/>
+      <c r="F177" s="10"/>
+      <c r="G177" s="10"/>
+      <c r="H177" s="10"/>
+      <c r="I177" s="10"/>
+      <c r="J177" s="10"/>
+      <c r="K177" s="10"/>
+      <c r="L177" s="5"/>
+    </row>
+    <row r="178" spans="2:12">
+      <c r="B178" s="4"/>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10"/>
+      <c r="E178" s="10"/>
+      <c r="F178" s="10"/>
+      <c r="G178" s="10"/>
+      <c r="H178" s="10"/>
+      <c r="I178" s="10"/>
+      <c r="J178" s="10"/>
+      <c r="K178" s="10"/>
+      <c r="L178" s="5"/>
+    </row>
+    <row r="179" spans="2:12">
+      <c r="B179" s="4"/>
+      <c r="C179" s="10"/>
+      <c r="D179" s="10"/>
+      <c r="E179" s="10"/>
+      <c r="F179" s="10"/>
+      <c r="G179" s="10"/>
+      <c r="H179" s="10"/>
+      <c r="I179" s="10"/>
+      <c r="J179" s="10"/>
+      <c r="K179" s="10"/>
+      <c r="L179" s="5"/>
+    </row>
+    <row r="180" spans="2:12">
+      <c r="B180" s="4"/>
+      <c r="C180" s="10"/>
+      <c r="D180" s="10"/>
+      <c r="E180" s="10"/>
+      <c r="F180" s="10"/>
+      <c r="G180" s="10"/>
+      <c r="H180" s="10"/>
+      <c r="I180" s="10"/>
+      <c r="J180" s="10"/>
+      <c r="K180" s="10"/>
+      <c r="L180" s="5"/>
+    </row>
+    <row r="181" spans="2:12">
+      <c r="B181" s="4"/>
+      <c r="C181" s="10"/>
+      <c r="D181" s="10"/>
+      <c r="E181" s="10"/>
+      <c r="F181" s="10"/>
+      <c r="G181" s="10"/>
+      <c r="H181" s="10"/>
+      <c r="I181" s="10"/>
+      <c r="J181" s="10"/>
+      <c r="K181" s="10"/>
+      <c r="L181" s="5"/>
+    </row>
+    <row r="182" spans="2:12">
+      <c r="B182" s="4"/>
+      <c r="C182" s="10"/>
+      <c r="D182" s="10"/>
+      <c r="E182" s="10"/>
+      <c r="F182" s="10"/>
+      <c r="G182" s="10"/>
+      <c r="H182" s="10"/>
+      <c r="I182" s="10"/>
+      <c r="J182" s="10"/>
+      <c r="K182" s="10"/>
+      <c r="L182" s="5"/>
+    </row>
+    <row r="183" spans="2:12">
+      <c r="B183" s="4"/>
+      <c r="C183" s="10"/>
+      <c r="D183" s="10"/>
+      <c r="E183" s="10"/>
+      <c r="F183" s="10"/>
+      <c r="G183" s="10"/>
+      <c r="H183" s="10"/>
+      <c r="I183" s="10"/>
+      <c r="J183" s="10"/>
+      <c r="K183" s="10"/>
+      <c r="L183" s="5"/>
+    </row>
+    <row r="184" spans="2:12">
+      <c r="B184" s="4"/>
+      <c r="C184" s="10"/>
+      <c r="D184" s="10"/>
+      <c r="E184" s="10"/>
+      <c r="F184" s="10"/>
+      <c r="G184" s="10"/>
+      <c r="H184" s="10"/>
+      <c r="I184" s="10"/>
+      <c r="J184" s="10"/>
+      <c r="K184" s="10"/>
+      <c r="L184" s="5"/>
+    </row>
+    <row r="185" spans="2:12">
+      <c r="B185" s="4"/>
+      <c r="C185" s="10"/>
+      <c r="D185" s="10"/>
+      <c r="E185" s="10"/>
+      <c r="F185" s="10"/>
+      <c r="G185" s="10"/>
+      <c r="H185" s="10"/>
+      <c r="I185" s="10"/>
+      <c r="J185" s="10"/>
+      <c r="K185" s="10"/>
+      <c r="L185" s="5"/>
+    </row>
+    <row r="186" spans="2:12">
+      <c r="B186" s="4"/>
+      <c r="C186" s="10"/>
+      <c r="D186" s="10"/>
+      <c r="E186" s="10"/>
+      <c r="F186" s="10"/>
+      <c r="G186" s="10"/>
+      <c r="H186" s="10"/>
+      <c r="I186" s="10"/>
+      <c r="J186" s="10"/>
+      <c r="K186" s="10"/>
+      <c r="L186" s="5"/>
+    </row>
+    <row r="187" spans="2:12">
+      <c r="B187" s="4"/>
+      <c r="C187" s="10"/>
+      <c r="D187" s="10"/>
+      <c r="E187" s="10"/>
+      <c r="F187" s="10"/>
+      <c r="G187" s="10"/>
+      <c r="H187" s="10"/>
+      <c r="I187" s="10"/>
+      <c r="J187" s="10"/>
+      <c r="K187" s="10"/>
+      <c r="L187" s="5"/>
+    </row>
+    <row r="188" spans="2:12">
+      <c r="B188" s="4"/>
+      <c r="C188" s="10"/>
+      <c r="D188" s="10"/>
+      <c r="E188" s="10"/>
+      <c r="F188" s="10"/>
+      <c r="G188" s="10"/>
+      <c r="H188" s="10"/>
+      <c r="I188" s="10"/>
+      <c r="J188" s="10"/>
+      <c r="K188" s="10"/>
+      <c r="L188" s="5"/>
+    </row>
+    <row r="189" spans="2:12">
+      <c r="B189" s="4"/>
+      <c r="C189" s="10"/>
+      <c r="D189" s="10"/>
+      <c r="E189" s="10"/>
+      <c r="F189" s="10"/>
+      <c r="G189" s="10"/>
+      <c r="H189" s="10"/>
+      <c r="I189" s="10"/>
+      <c r="J189" s="10"/>
+      <c r="K189" s="10"/>
+      <c r="L189" s="5"/>
+    </row>
+    <row r="190" spans="2:12">
+      <c r="B190" s="4"/>
+      <c r="C190" s="10"/>
+      <c r="D190" s="10"/>
+      <c r="E190" s="10"/>
+      <c r="F190" s="10"/>
+      <c r="G190" s="10"/>
+      <c r="H190" s="10"/>
+      <c r="I190" s="10"/>
+      <c r="J190" s="10"/>
+      <c r="K190" s="10"/>
+      <c r="L190" s="5"/>
+    </row>
+    <row r="191" spans="2:12">
+      <c r="B191" s="4"/>
+      <c r="C191" s="10"/>
+      <c r="D191" s="10"/>
+      <c r="E191" s="10"/>
+      <c r="F191" s="10"/>
+      <c r="G191" s="10"/>
+      <c r="H191" s="10"/>
+      <c r="I191" s="10"/>
+      <c r="J191" s="10"/>
+      <c r="K191" s="10"/>
+      <c r="L191" s="5"/>
+    </row>
+    <row r="192" spans="2:12">
+      <c r="B192" s="4"/>
+      <c r="C192" s="10"/>
+      <c r="D192" s="10"/>
+      <c r="E192" s="10"/>
+      <c r="F192" s="10"/>
+      <c r="G192" s="10"/>
+      <c r="H192" s="10"/>
+      <c r="I192" s="10"/>
+      <c r="J192" s="10"/>
+      <c r="K192" s="10"/>
+      <c r="L192" s="5"/>
+    </row>
+    <row r="193" spans="2:12">
+      <c r="B193" s="4"/>
+      <c r="C193" s="10"/>
+      <c r="D193" s="10"/>
+      <c r="E193" s="10"/>
+      <c r="F193" s="10"/>
+      <c r="G193" s="10"/>
+      <c r="H193" s="10"/>
+      <c r="I193" s="10"/>
+      <c r="J193" s="10"/>
+      <c r="K193" s="10"/>
+      <c r="L193" s="5"/>
+    </row>
+    <row r="194" spans="2:12">
+      <c r="B194" s="4"/>
+      <c r="C194" s="10"/>
+      <c r="D194" s="10"/>
+      <c r="E194" s="10"/>
+      <c r="F194" s="10"/>
+      <c r="G194" s="10"/>
+      <c r="H194" s="10"/>
+      <c r="I194" s="10"/>
+      <c r="J194" s="10"/>
+      <c r="K194" s="10"/>
+      <c r="L194" s="5"/>
+    </row>
+    <row r="195" spans="2:12">
+      <c r="B195" s="4"/>
+      <c r="C195" s="10"/>
+      <c r="D195" s="10"/>
+      <c r="E195" s="10"/>
+      <c r="F195" s="10"/>
+      <c r="G195" s="10"/>
+      <c r="H195" s="10"/>
+      <c r="I195" s="10"/>
+      <c r="J195" s="10"/>
+      <c r="K195" s="10"/>
+      <c r="L195" s="5"/>
+    </row>
+    <row r="196" spans="2:12">
+      <c r="B196" s="4"/>
+      <c r="C196" s="10"/>
+      <c r="D196" s="10"/>
+      <c r="E196" s="10"/>
+      <c r="F196" s="10"/>
+      <c r="G196" s="10"/>
+      <c r="H196" s="10"/>
+      <c r="I196" s="10"/>
+      <c r="J196" s="10"/>
+      <c r="K196" s="10"/>
+      <c r="L196" s="5"/>
+    </row>
+    <row r="197" spans="2:12">
+      <c r="B197" s="4"/>
+      <c r="C197" s="10"/>
+      <c r="D197" s="10"/>
+      <c r="E197" s="10"/>
+      <c r="F197" s="10"/>
+      <c r="G197" s="10"/>
+      <c r="H197" s="10"/>
+      <c r="I197" s="10"/>
+      <c r="J197" s="10"/>
+      <c r="K197" s="10"/>
+      <c r="L197" s="5"/>
+    </row>
+    <row r="198" spans="2:12">
+      <c r="B198" s="4"/>
+      <c r="C198" s="10"/>
+      <c r="D198" s="10"/>
+      <c r="E198" s="10"/>
+      <c r="F198" s="10"/>
+      <c r="G198" s="10"/>
+      <c r="H198" s="10"/>
+      <c r="I198" s="10"/>
+      <c r="J198" s="10"/>
+      <c r="K198" s="10"/>
+      <c r="L198" s="5"/>
+    </row>
+    <row r="199" spans="2:12">
+      <c r="B199" s="4"/>
+      <c r="C199" s="10"/>
+      <c r="D199" s="10"/>
+      <c r="E199" s="10"/>
+      <c r="F199" s="10"/>
+      <c r="G199" s="10"/>
+      <c r="H199" s="10"/>
+      <c r="I199" s="10"/>
+      <c r="J199" s="10"/>
+      <c r="K199" s="10"/>
+      <c r="L199" s="5"/>
+    </row>
+    <row r="200" spans="2:12">
+      <c r="B200" s="7"/>
+      <c r="C200" s="8"/>
+      <c r="D200" s="8"/>
+      <c r="E200" s="8"/>
+      <c r="F200" s="8"/>
+      <c r="G200" s="8"/>
+      <c r="H200" s="8"/>
+      <c r="I200" s="8"/>
+      <c r="J200" s="8"/>
+      <c r="K200" s="8"/>
+      <c r="L200" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Handling Ambiguous Column Names
</commit_message>
<xml_diff>
--- a/11.Joining-Multiple-Tables/Joining-Multiple-Tables.xlsx
+++ b/11.Joining-Multiple-Tables/Joining-Multiple-Tables.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\oracle\11.Joining-Multiple-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE6C859-455C-40E0-B270-3D6E6167E3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE960B2C-9AE9-4FB9-BADE-0BFD0959D5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29130" yWindow="180" windowWidth="25530" windowHeight="13155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29130" yWindow="180" windowWidth="25530" windowHeight="13155" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oracle SQL Join Types" sheetId="1" r:id="rId1"/>
     <sheet name="Natural Join" sheetId="2" r:id="rId2"/>
     <sheet name="Join with the USING Clause" sheetId="3" r:id="rId3"/>
+    <sheet name="Handling Ambiguous Column Names" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
   <si>
     <t>oracle</t>
     <phoneticPr fontId="1"/>
@@ -322,6 +323,479 @@
   </si>
   <si>
     <t>when joining 2 tables</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT first_name, last_name, department_name, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>manager_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> FROM employees JOIN departments</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We will get the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">column ambiguously </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>defined error because the manager ID column exists</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>more than one table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and the SQL engine doesn't know which one we want to display because</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the data in these columns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">may be different </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>than each other</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT first_name, last_name, department_name, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e.manager_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> FROM employees </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> JOIN departments </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>first_name, last_name, department_name, d.manager_id FROM employees e JOIN departments d</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We have to write table alias for a column </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">only </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>if that column exists in more than one table. Otherwise</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">it is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>optional</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and that won't change the result</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT first_name, last_name, department_name, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>departments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.manager_id FROM employees e JOIN departments </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If we assign an alias to a table, we can not use its name before the column name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>USING(manager_id);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>can not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> give aliases to columns that we</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> used </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">in the USING clause or NATURAL joins </t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT first_name, last_name, department_name, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>departments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.manager_id FROM employees e JOIN departments</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SELECT first_name, last_name, department_name, manager_id FROM employees e JOIN departments</t>
+  </si>
+  <si>
+    <r>
+      <t>USING(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>manager_id);</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">we </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">can not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>give aliases to columns that we used in the USING clause</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>using table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> aliases increases performance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. If we do not specify table alias for columns the database has to find which column belongs to which table when joining</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">the tables but in case we have a lot of tables to be joined, this will take some extra time from the CPU. So if we write column aliases for all columns, this time the </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">database will know column belongs to which table in advance and this might have a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slightly better performance</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -460,7 +934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -471,8 +945,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -945,6 +1417,478 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{386DE29F-D3B0-9ECA-D040-3AB46810E762}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="758825" y="4673600"/>
+          <a:ext cx="9652000" cy="4755030"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>59971</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{338DEE8C-7817-70F4-DBCE-A89F611603C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="10410824"/>
+          <a:ext cx="7997825" cy="2679347"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>46969</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="図 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FEFE0C1-9EA9-2AEF-8293-721D162CCC16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="14230349"/>
+          <a:ext cx="7477125" cy="8444845"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>50708</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="図 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86AC256C-6A51-6D3D-87D8-92382B3BB971}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="796925" y="23856950"/>
+          <a:ext cx="7223125" cy="7972333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>50742</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="図 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7217696E-2AFA-15D3-FEB3-BF30831A044A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="32981900"/>
+          <a:ext cx="7505700" cy="2276417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>587375</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>57170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="図 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07DBAC13-A7A8-E689-B0D9-5F50EE59AF78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="790575" y="36452174"/>
+          <a:ext cx="7683500" cy="2466996"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="直線矢印コネクタ 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0A61505-0846-4D84-DF5A-666BF154265A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2085975" y="36061650"/>
+          <a:ext cx="10106025" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="直線矢印コネクタ 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34967578-CF87-E1F8-C912-BAC840CB110E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2066925" y="36068000"/>
+          <a:ext cx="2901950" cy="184150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>188</xdr:row>
+      <xdr:rowOff>83225</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="図 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{701B6F55-3091-5B52-D928-C695A5A6D7F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="40109774"/>
+          <a:ext cx="7648575" cy="2496226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="直線矢印コネクタ 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A0A92F-BE17-7432-EAB2-34BAAE746014}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2066925" y="39738300"/>
+          <a:ext cx="10829925" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2093,8 +3037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6573E67-C2FE-449F-BFF9-38AE202CC8A7}">
   <dimension ref="B3:V132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y96" sqref="Y96"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -2195,7 +3139,7 @@
     </row>
     <row r="15" spans="2:13">
       <c r="B15" s="4"/>
-      <c r="D15" s="10" t="s">
+      <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="M15" s="5"/>
@@ -2243,150 +3187,66 @@
       <c r="B42" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="2:10">
       <c r="B43" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="2:10">
       <c r="B44" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
       <c r="J44" s="5"/>
     </row>
     <row r="45" spans="2:10">
       <c r="B45" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
       <c r="J45" s="5"/>
     </row>
     <row r="46" spans="2:10">
       <c r="B46" s="4"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
       <c r="J46" s="5"/>
     </row>
     <row r="47" spans="2:10">
       <c r="B47" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
       <c r="J47" s="5"/>
     </row>
     <row r="48" spans="2:10">
       <c r="B48" s="4"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
       <c r="J48" s="5"/>
     </row>
     <row r="49" spans="2:22">
       <c r="B49" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
       <c r="J49" s="5"/>
     </row>
     <row r="50" spans="2:22">
       <c r="B50" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
       <c r="J50" s="5"/>
     </row>
     <row r="51" spans="2:22">
       <c r="B51" s="4"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
       <c r="J51" s="5"/>
     </row>
     <row r="52" spans="2:22">
       <c r="B52" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
       <c r="J52" s="5"/>
     </row>
     <row r="53" spans="2:22">
       <c r="B53" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
       <c r="J53" s="5"/>
     </row>
     <row r="54" spans="2:22">
@@ -2427,23 +3287,6 @@
       <c r="B58" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="11"/>
-      <c r="S58" s="11"/>
       <c r="T58" s="5"/>
       <c r="U58" t="s">
         <v>28</v>
@@ -2454,23 +3297,6 @@
     </row>
     <row r="59" spans="2:22">
       <c r="B59" s="4"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-      <c r="L59" s="11"/>
-      <c r="M59" s="11"/>
-      <c r="N59" s="11"/>
-      <c r="O59" s="11"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="11"/>
-      <c r="S59" s="11"/>
       <c r="T59" s="5"/>
       <c r="V59" t="s">
         <v>41</v>
@@ -2478,23 +3304,6 @@
     </row>
     <row r="60" spans="2:22">
       <c r="B60" s="4"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
-      <c r="N60" s="11"/>
-      <c r="O60" s="11"/>
-      <c r="P60" s="11"/>
-      <c r="Q60" s="11"/>
-      <c r="R60" s="11"/>
-      <c r="S60" s="11"/>
       <c r="T60" s="5"/>
       <c r="V60" t="s">
         <v>42</v>
@@ -2502,149 +3311,30 @@
     </row>
     <row r="61" spans="2:22">
       <c r="B61" s="4"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="11"/>
-      <c r="M61" s="11"/>
-      <c r="N61" s="11"/>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
-      <c r="Q61" s="11"/>
-      <c r="R61" s="11"/>
-      <c r="S61" s="11"/>
       <c r="T61" s="5"/>
     </row>
     <row r="62" spans="2:22">
       <c r="B62" s="4"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11"/>
-      <c r="M62" s="11"/>
-      <c r="N62" s="11"/>
-      <c r="O62" s="11"/>
-      <c r="P62" s="11"/>
-      <c r="Q62" s="11"/>
-      <c r="R62" s="11"/>
-      <c r="S62" s="11"/>
       <c r="T62" s="5"/>
     </row>
     <row r="63" spans="2:22">
       <c r="B63" s="4"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-      <c r="L63" s="11"/>
-      <c r="M63" s="11"/>
-      <c r="N63" s="11"/>
-      <c r="O63" s="11"/>
-      <c r="P63" s="11"/>
-      <c r="Q63" s="11"/>
-      <c r="R63" s="11"/>
-      <c r="S63" s="11"/>
       <c r="T63" s="5"/>
     </row>
     <row r="64" spans="2:22">
       <c r="B64" s="4"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11"/>
-      <c r="N64" s="11"/>
-      <c r="O64" s="11"/>
-      <c r="P64" s="11"/>
-      <c r="Q64" s="11"/>
-      <c r="R64" s="11"/>
-      <c r="S64" s="11"/>
       <c r="T64" s="5"/>
     </row>
     <row r="65" spans="2:22">
       <c r="B65" s="4"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
-      <c r="L65" s="11"/>
-      <c r="M65" s="11"/>
-      <c r="N65" s="11"/>
-      <c r="O65" s="11"/>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="11"/>
-      <c r="R65" s="11"/>
-      <c r="S65" s="11"/>
       <c r="T65" s="5"/>
     </row>
     <row r="66" spans="2:22">
       <c r="B66" s="4"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
-      <c r="L66" s="11"/>
-      <c r="M66" s="11"/>
-      <c r="N66" s="11"/>
-      <c r="O66" s="11"/>
-      <c r="P66" s="11"/>
-      <c r="Q66" s="11"/>
-      <c r="R66" s="11"/>
-      <c r="S66" s="11"/>
       <c r="T66" s="5"/>
     </row>
     <row r="67" spans="2:22">
       <c r="B67" s="4"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
-      <c r="L67" s="11"/>
-      <c r="M67" s="11"/>
-      <c r="N67" s="11"/>
-      <c r="O67" s="11"/>
-      <c r="P67" s="11"/>
-      <c r="Q67" s="11"/>
-      <c r="R67" s="11"/>
-      <c r="S67" s="11"/>
       <c r="T67" s="5"/>
       <c r="U67" t="s">
         <v>28</v>
@@ -2655,485 +3345,94 @@
     </row>
     <row r="68" spans="2:22">
       <c r="B68" s="4"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-      <c r="L68" s="11"/>
-      <c r="M68" s="11"/>
-      <c r="N68" s="11"/>
-      <c r="O68" s="11"/>
-      <c r="P68" s="11"/>
-      <c r="Q68" s="11"/>
-      <c r="R68" s="11"/>
-      <c r="S68" s="11"/>
       <c r="T68" s="5"/>
     </row>
     <row r="69" spans="2:22">
       <c r="B69" s="4"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="11"/>
-      <c r="N69" s="11"/>
-      <c r="O69" s="11"/>
-      <c r="P69" s="11"/>
-      <c r="Q69" s="11"/>
-      <c r="R69" s="11"/>
-      <c r="S69" s="11"/>
       <c r="T69" s="5"/>
     </row>
     <row r="70" spans="2:22">
       <c r="B70" s="4"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="11"/>
-      <c r="O70" s="11"/>
-      <c r="P70" s="11"/>
-      <c r="Q70" s="11"/>
-      <c r="R70" s="11"/>
-      <c r="S70" s="11"/>
       <c r="T70" s="5"/>
     </row>
     <row r="71" spans="2:22">
       <c r="B71" s="4"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
-      <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
-      <c r="N71" s="11"/>
-      <c r="O71" s="11"/>
-      <c r="P71" s="11"/>
-      <c r="Q71" s="11"/>
-      <c r="R71" s="11"/>
-      <c r="S71" s="11"/>
       <c r="T71" s="5"/>
     </row>
     <row r="72" spans="2:22">
       <c r="B72" s="4"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
-      <c r="K72" s="11"/>
-      <c r="L72" s="11"/>
-      <c r="M72" s="11"/>
-      <c r="N72" s="11"/>
-      <c r="O72" s="11"/>
-      <c r="P72" s="11"/>
-      <c r="Q72" s="11"/>
-      <c r="R72" s="11"/>
-      <c r="S72" s="11"/>
       <c r="T72" s="5"/>
     </row>
     <row r="73" spans="2:22">
       <c r="B73" s="4"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="11"/>
-      <c r="K73" s="11"/>
-      <c r="L73" s="11"/>
-      <c r="M73" s="11"/>
-      <c r="N73" s="11"/>
-      <c r="O73" s="11"/>
-      <c r="P73" s="11"/>
-      <c r="Q73" s="11"/>
-      <c r="R73" s="11"/>
-      <c r="S73" s="11"/>
       <c r="T73" s="5"/>
     </row>
     <row r="74" spans="2:22">
       <c r="B74" s="4"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="11"/>
-      <c r="L74" s="11"/>
-      <c r="M74" s="11"/>
-      <c r="N74" s="11"/>
-      <c r="O74" s="11"/>
-      <c r="P74" s="11"/>
-      <c r="Q74" s="11"/>
-      <c r="R74" s="11"/>
-      <c r="S74" s="11"/>
       <c r="T74" s="5"/>
     </row>
     <row r="75" spans="2:22">
       <c r="B75" s="4"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="11"/>
-      <c r="K75" s="11"/>
-      <c r="L75" s="11"/>
-      <c r="M75" s="11"/>
-      <c r="N75" s="11"/>
-      <c r="O75" s="11"/>
-      <c r="P75" s="11"/>
-      <c r="Q75" s="11"/>
-      <c r="R75" s="11"/>
-      <c r="S75" s="11"/>
       <c r="T75" s="5"/>
     </row>
     <row r="76" spans="2:22">
       <c r="B76" s="4"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="11"/>
-      <c r="K76" s="11"/>
-      <c r="L76" s="11"/>
-      <c r="M76" s="11"/>
-      <c r="N76" s="11"/>
-      <c r="O76" s="11"/>
-      <c r="P76" s="11"/>
-      <c r="Q76" s="11"/>
-      <c r="R76" s="11"/>
-      <c r="S76" s="11"/>
       <c r="T76" s="5"/>
     </row>
     <row r="77" spans="2:22">
       <c r="B77" s="4"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="11"/>
-      <c r="L77" s="11"/>
-      <c r="M77" s="11"/>
-      <c r="N77" s="11"/>
-      <c r="O77" s="11"/>
-      <c r="P77" s="11"/>
-      <c r="Q77" s="11"/>
-      <c r="R77" s="11"/>
-      <c r="S77" s="11"/>
       <c r="T77" s="5"/>
     </row>
     <row r="78" spans="2:22">
       <c r="B78" s="4"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="11"/>
-      <c r="K78" s="11"/>
-      <c r="L78" s="11"/>
-      <c r="M78" s="11"/>
-      <c r="N78" s="11"/>
-      <c r="O78" s="11"/>
-      <c r="P78" s="11"/>
-      <c r="Q78" s="11"/>
-      <c r="R78" s="11"/>
-      <c r="S78" s="11"/>
       <c r="T78" s="5"/>
     </row>
     <row r="79" spans="2:22">
       <c r="B79" s="4"/>
-      <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="11"/>
-      <c r="K79" s="11"/>
-      <c r="L79" s="11"/>
-      <c r="M79" s="11"/>
-      <c r="N79" s="11"/>
-      <c r="O79" s="11"/>
-      <c r="P79" s="11"/>
-      <c r="Q79" s="11"/>
-      <c r="R79" s="11"/>
-      <c r="S79" s="11"/>
       <c r="T79" s="5"/>
     </row>
     <row r="80" spans="2:22">
       <c r="B80" s="4"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
-      <c r="I80" s="11"/>
-      <c r="J80" s="11"/>
-      <c r="K80" s="11"/>
-      <c r="L80" s="11"/>
-      <c r="M80" s="11"/>
-      <c r="N80" s="11"/>
-      <c r="O80" s="11"/>
-      <c r="P80" s="11"/>
-      <c r="Q80" s="11"/>
-      <c r="R80" s="11"/>
-      <c r="S80" s="11"/>
       <c r="T80" s="5"/>
     </row>
     <row r="81" spans="2:22">
       <c r="B81" s="4"/>
-      <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="11"/>
-      <c r="J81" s="11"/>
-      <c r="K81" s="11"/>
-      <c r="L81" s="11"/>
-      <c r="M81" s="11"/>
-      <c r="N81" s="11"/>
-      <c r="O81" s="11"/>
-      <c r="P81" s="11"/>
-      <c r="Q81" s="11"/>
-      <c r="R81" s="11"/>
-      <c r="S81" s="11"/>
       <c r="T81" s="5"/>
     </row>
     <row r="82" spans="2:22">
       <c r="B82" s="4"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
-      <c r="J82" s="11"/>
-      <c r="K82" s="11"/>
-      <c r="L82" s="11"/>
-      <c r="M82" s="11"/>
-      <c r="N82" s="11"/>
-      <c r="O82" s="11"/>
-      <c r="P82" s="11"/>
-      <c r="Q82" s="11"/>
-      <c r="R82" s="11"/>
-      <c r="S82" s="11"/>
       <c r="T82" s="5"/>
     </row>
     <row r="83" spans="2:22">
       <c r="B83" s="4"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="11"/>
-      <c r="L83" s="11"/>
-      <c r="M83" s="11"/>
-      <c r="N83" s="11"/>
-      <c r="O83" s="11"/>
-      <c r="P83" s="11"/>
-      <c r="Q83" s="11"/>
-      <c r="R83" s="11"/>
-      <c r="S83" s="11"/>
       <c r="T83" s="5"/>
     </row>
     <row r="84" spans="2:22">
       <c r="B84" s="4"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="11"/>
-      <c r="K84" s="11"/>
-      <c r="L84" s="11"/>
-      <c r="M84" s="11"/>
-      <c r="N84" s="11"/>
-      <c r="O84" s="11"/>
-      <c r="P84" s="11"/>
-      <c r="Q84" s="11"/>
-      <c r="R84" s="11"/>
-      <c r="S84" s="11"/>
       <c r="T84" s="5"/>
     </row>
     <row r="85" spans="2:22">
       <c r="B85" s="4"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
-      <c r="H85" s="11"/>
-      <c r="I85" s="11"/>
-      <c r="J85" s="11"/>
-      <c r="K85" s="11"/>
-      <c r="L85" s="11"/>
-      <c r="M85" s="11"/>
-      <c r="N85" s="11"/>
-      <c r="O85" s="11"/>
-      <c r="P85" s="11"/>
-      <c r="Q85" s="11"/>
-      <c r="R85" s="11"/>
-      <c r="S85" s="11"/>
       <c r="T85" s="5"/>
     </row>
     <row r="86" spans="2:22">
       <c r="B86" s="4"/>
-      <c r="C86" s="11"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
-      <c r="H86" s="11"/>
-      <c r="I86" s="11"/>
-      <c r="J86" s="11"/>
-      <c r="K86" s="11"/>
-      <c r="L86" s="11"/>
-      <c r="M86" s="11"/>
-      <c r="N86" s="11"/>
-      <c r="O86" s="11"/>
-      <c r="P86" s="11"/>
-      <c r="Q86" s="11"/>
-      <c r="R86" s="11"/>
-      <c r="S86" s="11"/>
       <c r="T86" s="5"/>
     </row>
     <row r="87" spans="2:22">
       <c r="B87" s="4"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="11"/>
-      <c r="K87" s="11"/>
-      <c r="L87" s="11"/>
-      <c r="M87" s="11"/>
-      <c r="N87" s="11"/>
-      <c r="O87" s="11"/>
-      <c r="P87" s="11"/>
-      <c r="Q87" s="11"/>
-      <c r="R87" s="11"/>
-      <c r="S87" s="11"/>
       <c r="T87" s="5"/>
     </row>
     <row r="88" spans="2:22">
       <c r="B88" s="4"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
-      <c r="G88" s="11"/>
-      <c r="H88" s="11"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="11"/>
-      <c r="K88" s="11"/>
-      <c r="L88" s="11"/>
-      <c r="M88" s="11"/>
-      <c r="N88" s="11"/>
-      <c r="O88" s="11"/>
-      <c r="P88" s="11"/>
-      <c r="Q88" s="11"/>
-      <c r="R88" s="11"/>
-      <c r="S88" s="11"/>
       <c r="T88" s="5"/>
     </row>
     <row r="89" spans="2:22">
       <c r="B89" s="4"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
-      <c r="L89" s="11"/>
-      <c r="M89" s="11"/>
-      <c r="N89" s="11"/>
-      <c r="O89" s="11"/>
-      <c r="P89" s="11"/>
-      <c r="Q89" s="11"/>
-      <c r="R89" s="11"/>
-      <c r="S89" s="11"/>
       <c r="T89" s="5"/>
     </row>
     <row r="90" spans="2:22">
       <c r="B90" s="4"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="11"/>
-      <c r="K90" s="11"/>
-      <c r="L90" s="11"/>
-      <c r="M90" s="11"/>
-      <c r="N90" s="11"/>
-      <c r="O90" s="11"/>
-      <c r="P90" s="11"/>
-      <c r="Q90" s="11"/>
-      <c r="R90" s="11"/>
-      <c r="S90" s="11"/>
       <c r="T90" s="5"/>
     </row>
     <row r="91" spans="2:22">
@@ -3184,23 +3483,6 @@
       <c r="B95" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="11"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="11"/>
-      <c r="J95" s="11"/>
-      <c r="K95" s="11"/>
-      <c r="L95" s="11"/>
-      <c r="M95" s="11"/>
-      <c r="N95" s="11"/>
-      <c r="O95" s="11"/>
-      <c r="P95" s="11"/>
-      <c r="Q95" s="11"/>
-      <c r="R95" s="11"/>
-      <c r="S95" s="11"/>
       <c r="T95" s="5"/>
       <c r="U95" t="s">
         <v>28</v>
@@ -3211,23 +3493,6 @@
     </row>
     <row r="96" spans="2:22">
       <c r="B96" s="4"/>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="11"/>
-      <c r="K96" s="11"/>
-      <c r="L96" s="11"/>
-      <c r="M96" s="11"/>
-      <c r="N96" s="11"/>
-      <c r="O96" s="11"/>
-      <c r="P96" s="11"/>
-      <c r="Q96" s="11"/>
-      <c r="R96" s="11"/>
-      <c r="S96" s="11"/>
       <c r="T96" s="5"/>
       <c r="V96" t="s">
         <v>45</v>
@@ -3235,737 +3500,142 @@
     </row>
     <row r="97" spans="2:20">
       <c r="B97" s="4"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="11"/>
-      <c r="K97" s="11"/>
-      <c r="L97" s="11"/>
-      <c r="M97" s="11"/>
-      <c r="N97" s="11"/>
-      <c r="O97" s="11"/>
-      <c r="P97" s="11"/>
-      <c r="Q97" s="11"/>
-      <c r="R97" s="11"/>
-      <c r="S97" s="11"/>
       <c r="T97" s="5"/>
     </row>
     <row r="98" spans="2:20">
       <c r="B98" s="4"/>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
-      <c r="K98" s="11"/>
-      <c r="L98" s="11"/>
-      <c r="M98" s="11"/>
-      <c r="N98" s="11"/>
-      <c r="O98" s="11"/>
-      <c r="P98" s="11"/>
-      <c r="Q98" s="11"/>
-      <c r="R98" s="11"/>
-      <c r="S98" s="11"/>
       <c r="T98" s="5"/>
     </row>
     <row r="99" spans="2:20">
       <c r="B99" s="4"/>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="11"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="11"/>
-      <c r="K99" s="11"/>
-      <c r="L99" s="11"/>
-      <c r="M99" s="11"/>
-      <c r="N99" s="11"/>
-      <c r="O99" s="11"/>
-      <c r="P99" s="11"/>
-      <c r="Q99" s="11"/>
-      <c r="R99" s="11"/>
-      <c r="S99" s="11"/>
       <c r="T99" s="5"/>
     </row>
     <row r="100" spans="2:20">
       <c r="B100" s="4"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="11"/>
-      <c r="K100" s="11"/>
-      <c r="L100" s="11"/>
-      <c r="M100" s="11"/>
-      <c r="N100" s="11"/>
-      <c r="O100" s="11"/>
-      <c r="P100" s="11"/>
-      <c r="Q100" s="11"/>
-      <c r="R100" s="11"/>
-      <c r="S100" s="11"/>
       <c r="T100" s="5"/>
     </row>
     <row r="101" spans="2:20">
       <c r="B101" s="4"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
-      <c r="I101" s="11"/>
-      <c r="J101" s="11"/>
-      <c r="K101" s="11"/>
-      <c r="L101" s="11"/>
-      <c r="M101" s="11"/>
-      <c r="N101" s="11"/>
-      <c r="O101" s="11"/>
-      <c r="P101" s="11"/>
-      <c r="Q101" s="11"/>
-      <c r="R101" s="11"/>
-      <c r="S101" s="11"/>
       <c r="T101" s="5"/>
     </row>
     <row r="102" spans="2:20">
       <c r="B102" s="4"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
-      <c r="I102" s="11"/>
-      <c r="J102" s="11"/>
-      <c r="K102" s="11"/>
-      <c r="L102" s="11"/>
-      <c r="M102" s="11"/>
-      <c r="N102" s="11"/>
-      <c r="O102" s="11"/>
-      <c r="P102" s="11"/>
-      <c r="Q102" s="11"/>
-      <c r="R102" s="11"/>
-      <c r="S102" s="11"/>
       <c r="T102" s="5"/>
     </row>
     <row r="103" spans="2:20">
       <c r="B103" s="4"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="11"/>
-      <c r="K103" s="11"/>
-      <c r="L103" s="11"/>
-      <c r="M103" s="11"/>
-      <c r="N103" s="11"/>
-      <c r="O103" s="11"/>
-      <c r="P103" s="11"/>
-      <c r="Q103" s="11"/>
-      <c r="R103" s="11"/>
-      <c r="S103" s="11"/>
       <c r="T103" s="5"/>
     </row>
     <row r="104" spans="2:20">
       <c r="B104" s="4"/>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
-      <c r="G104" s="11"/>
-      <c r="H104" s="11"/>
-      <c r="I104" s="11"/>
-      <c r="J104" s="11"/>
-      <c r="K104" s="11"/>
-      <c r="L104" s="11"/>
-      <c r="M104" s="11"/>
-      <c r="N104" s="11"/>
-      <c r="O104" s="11"/>
-      <c r="P104" s="11"/>
-      <c r="Q104" s="11"/>
-      <c r="R104" s="11"/>
-      <c r="S104" s="11"/>
       <c r="T104" s="5"/>
     </row>
     <row r="105" spans="2:20">
       <c r="B105" s="4"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="11"/>
-      <c r="H105" s="11"/>
-      <c r="I105" s="11"/>
-      <c r="J105" s="11"/>
-      <c r="K105" s="11"/>
-      <c r="L105" s="11"/>
-      <c r="M105" s="11"/>
-      <c r="N105" s="11"/>
-      <c r="O105" s="11"/>
-      <c r="P105" s="11"/>
-      <c r="Q105" s="11"/>
-      <c r="R105" s="11"/>
-      <c r="S105" s="11"/>
       <c r="T105" s="5"/>
     </row>
     <row r="106" spans="2:20">
       <c r="B106" s="4"/>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="11"/>
-      <c r="I106" s="11"/>
-      <c r="J106" s="11"/>
-      <c r="K106" s="11"/>
-      <c r="L106" s="11"/>
-      <c r="M106" s="11"/>
-      <c r="N106" s="11"/>
-      <c r="O106" s="11"/>
-      <c r="P106" s="11"/>
-      <c r="Q106" s="11"/>
-      <c r="R106" s="11"/>
-      <c r="S106" s="11"/>
       <c r="T106" s="5"/>
     </row>
     <row r="107" spans="2:20">
       <c r="B107" s="4"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11"/>
-      <c r="G107" s="11"/>
-      <c r="H107" s="11"/>
-      <c r="I107" s="11"/>
-      <c r="J107" s="11"/>
-      <c r="K107" s="11"/>
-      <c r="L107" s="11"/>
-      <c r="M107" s="11"/>
-      <c r="N107" s="11"/>
-      <c r="O107" s="11"/>
-      <c r="P107" s="11"/>
-      <c r="Q107" s="11"/>
-      <c r="R107" s="11"/>
-      <c r="S107" s="11"/>
       <c r="T107" s="5"/>
     </row>
     <row r="108" spans="2:20">
       <c r="B108" s="4"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
-      <c r="G108" s="11"/>
-      <c r="H108" s="11"/>
-      <c r="I108" s="11"/>
-      <c r="J108" s="11"/>
-      <c r="K108" s="11"/>
-      <c r="L108" s="11"/>
-      <c r="M108" s="11"/>
-      <c r="N108" s="11"/>
-      <c r="O108" s="11"/>
-      <c r="P108" s="11"/>
-      <c r="Q108" s="11"/>
-      <c r="R108" s="11"/>
-      <c r="S108" s="11"/>
       <c r="T108" s="5"/>
     </row>
     <row r="109" spans="2:20">
       <c r="B109" s="4"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
-      <c r="G109" s="11"/>
-      <c r="H109" s="11"/>
-      <c r="I109" s="11"/>
-      <c r="J109" s="11"/>
-      <c r="K109" s="11"/>
-      <c r="L109" s="11"/>
-      <c r="M109" s="11"/>
-      <c r="N109" s="11"/>
-      <c r="O109" s="11"/>
-      <c r="P109" s="11"/>
-      <c r="Q109" s="11"/>
-      <c r="R109" s="11"/>
-      <c r="S109" s="11"/>
       <c r="T109" s="5"/>
     </row>
     <row r="110" spans="2:20">
       <c r="B110" s="4"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
-      <c r="G110" s="11"/>
-      <c r="H110" s="11"/>
-      <c r="I110" s="11"/>
-      <c r="J110" s="11"/>
-      <c r="K110" s="11"/>
-      <c r="L110" s="11"/>
-      <c r="M110" s="11"/>
-      <c r="N110" s="11"/>
-      <c r="O110" s="11"/>
-      <c r="P110" s="11"/>
-      <c r="Q110" s="11"/>
-      <c r="R110" s="11"/>
-      <c r="S110" s="11"/>
       <c r="T110" s="5"/>
     </row>
     <row r="111" spans="2:20">
       <c r="B111" s="4"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11"/>
-      <c r="G111" s="11"/>
-      <c r="H111" s="11"/>
-      <c r="I111" s="11"/>
-      <c r="J111" s="11"/>
-      <c r="K111" s="11"/>
-      <c r="L111" s="11"/>
-      <c r="M111" s="11"/>
-      <c r="N111" s="11"/>
-      <c r="O111" s="11"/>
-      <c r="P111" s="11"/>
-      <c r="Q111" s="11"/>
-      <c r="R111" s="11"/>
-      <c r="S111" s="11"/>
       <c r="T111" s="5"/>
     </row>
     <row r="112" spans="2:20">
       <c r="B112" s="4"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
-      <c r="G112" s="11"/>
-      <c r="H112" s="11"/>
-      <c r="I112" s="11"/>
-      <c r="J112" s="11"/>
-      <c r="K112" s="11"/>
-      <c r="L112" s="11"/>
-      <c r="M112" s="11"/>
-      <c r="N112" s="11"/>
-      <c r="O112" s="11"/>
-      <c r="P112" s="11"/>
-      <c r="Q112" s="11"/>
-      <c r="R112" s="11"/>
-      <c r="S112" s="11"/>
       <c r="T112" s="5"/>
     </row>
     <row r="113" spans="2:20">
       <c r="B113" s="4"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
-      <c r="G113" s="11"/>
-      <c r="H113" s="11"/>
-      <c r="I113" s="11"/>
-      <c r="J113" s="11"/>
-      <c r="K113" s="11"/>
-      <c r="L113" s="11"/>
-      <c r="M113" s="11"/>
-      <c r="N113" s="11"/>
-      <c r="O113" s="11"/>
-      <c r="P113" s="11"/>
-      <c r="Q113" s="11"/>
-      <c r="R113" s="11"/>
-      <c r="S113" s="11"/>
       <c r="T113" s="5"/>
     </row>
     <row r="114" spans="2:20">
       <c r="B114" s="4"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
-      <c r="G114" s="11"/>
-      <c r="H114" s="11"/>
-      <c r="I114" s="11"/>
-      <c r="J114" s="11"/>
-      <c r="K114" s="11"/>
-      <c r="L114" s="11"/>
-      <c r="M114" s="11"/>
-      <c r="N114" s="11"/>
-      <c r="O114" s="11"/>
-      <c r="P114" s="11"/>
-      <c r="Q114" s="11"/>
-      <c r="R114" s="11"/>
-      <c r="S114" s="11"/>
       <c r="T114" s="5"/>
     </row>
     <row r="115" spans="2:20">
       <c r="B115" s="4"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
-      <c r="G115" s="11"/>
-      <c r="H115" s="11"/>
-      <c r="I115" s="11"/>
-      <c r="J115" s="11"/>
-      <c r="K115" s="11"/>
-      <c r="L115" s="11"/>
-      <c r="M115" s="11"/>
-      <c r="N115" s="11"/>
-      <c r="O115" s="11"/>
-      <c r="P115" s="11"/>
-      <c r="Q115" s="11"/>
-      <c r="R115" s="11"/>
-      <c r="S115" s="11"/>
       <c r="T115" s="5"/>
     </row>
     <row r="116" spans="2:20">
       <c r="B116" s="4"/>
-      <c r="C116" s="11"/>
-      <c r="D116" s="11"/>
-      <c r="E116" s="11"/>
-      <c r="F116" s="11"/>
-      <c r="G116" s="11"/>
-      <c r="H116" s="11"/>
-      <c r="I116" s="11"/>
-      <c r="J116" s="11"/>
-      <c r="K116" s="11"/>
-      <c r="L116" s="11"/>
-      <c r="M116" s="11"/>
-      <c r="N116" s="11"/>
-      <c r="O116" s="11"/>
-      <c r="P116" s="11"/>
-      <c r="Q116" s="11"/>
-      <c r="R116" s="11"/>
-      <c r="S116" s="11"/>
       <c r="T116" s="5"/>
     </row>
     <row r="117" spans="2:20">
       <c r="B117" s="4"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
-      <c r="G117" s="11"/>
-      <c r="H117" s="11"/>
-      <c r="I117" s="11"/>
-      <c r="J117" s="11"/>
-      <c r="K117" s="11"/>
-      <c r="L117" s="11"/>
-      <c r="M117" s="11"/>
-      <c r="N117" s="11"/>
-      <c r="O117" s="11"/>
-      <c r="P117" s="11"/>
-      <c r="Q117" s="11"/>
-      <c r="R117" s="11"/>
-      <c r="S117" s="11"/>
       <c r="T117" s="5"/>
     </row>
     <row r="118" spans="2:20">
       <c r="B118" s="4"/>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
-      <c r="G118" s="11"/>
-      <c r="H118" s="11"/>
-      <c r="I118" s="11"/>
-      <c r="J118" s="11"/>
-      <c r="K118" s="11"/>
-      <c r="L118" s="11"/>
-      <c r="M118" s="11"/>
-      <c r="N118" s="11"/>
-      <c r="O118" s="11"/>
-      <c r="P118" s="11"/>
-      <c r="Q118" s="11"/>
-      <c r="R118" s="11"/>
-      <c r="S118" s="11"/>
       <c r="T118" s="5"/>
     </row>
     <row r="119" spans="2:20">
       <c r="B119" s="4"/>
-      <c r="C119" s="11"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
-      <c r="G119" s="11"/>
-      <c r="H119" s="11"/>
-      <c r="I119" s="11"/>
-      <c r="J119" s="11"/>
-      <c r="K119" s="11"/>
-      <c r="L119" s="11"/>
-      <c r="M119" s="11"/>
-      <c r="N119" s="11"/>
-      <c r="O119" s="11"/>
-      <c r="P119" s="11"/>
-      <c r="Q119" s="11"/>
-      <c r="R119" s="11"/>
-      <c r="S119" s="11"/>
       <c r="T119" s="5"/>
     </row>
     <row r="120" spans="2:20">
       <c r="B120" s="4"/>
-      <c r="C120" s="11"/>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11"/>
-      <c r="F120" s="11"/>
-      <c r="G120" s="11"/>
-      <c r="H120" s="11"/>
-      <c r="I120" s="11"/>
-      <c r="J120" s="11"/>
-      <c r="K120" s="11"/>
-      <c r="L120" s="11"/>
-      <c r="M120" s="11"/>
-      <c r="N120" s="11"/>
-      <c r="O120" s="11"/>
-      <c r="P120" s="11"/>
-      <c r="Q120" s="11"/>
-      <c r="R120" s="11"/>
-      <c r="S120" s="11"/>
       <c r="T120" s="5"/>
     </row>
     <row r="121" spans="2:20">
       <c r="B121" s="4"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
-      <c r="F121" s="11"/>
-      <c r="G121" s="11"/>
-      <c r="H121" s="11"/>
-      <c r="I121" s="11"/>
-      <c r="J121" s="11"/>
-      <c r="K121" s="11"/>
-      <c r="L121" s="11"/>
-      <c r="M121" s="11"/>
-      <c r="N121" s="11"/>
-      <c r="O121" s="11"/>
-      <c r="P121" s="11"/>
-      <c r="Q121" s="11"/>
-      <c r="R121" s="11"/>
-      <c r="S121" s="11"/>
       <c r="T121" s="5"/>
     </row>
     <row r="122" spans="2:20">
       <c r="B122" s="4"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
-      <c r="F122" s="11"/>
-      <c r="G122" s="11"/>
-      <c r="H122" s="11"/>
-      <c r="I122" s="11"/>
-      <c r="J122" s="11"/>
-      <c r="K122" s="11"/>
-      <c r="L122" s="11"/>
-      <c r="M122" s="11"/>
-      <c r="N122" s="11"/>
-      <c r="O122" s="11"/>
-      <c r="P122" s="11"/>
-      <c r="Q122" s="11"/>
-      <c r="R122" s="11"/>
-      <c r="S122" s="11"/>
       <c r="T122" s="5"/>
     </row>
     <row r="123" spans="2:20">
       <c r="B123" s="4"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
-      <c r="F123" s="11"/>
-      <c r="G123" s="11"/>
-      <c r="H123" s="11"/>
-      <c r="I123" s="11"/>
-      <c r="J123" s="11"/>
-      <c r="K123" s="11"/>
-      <c r="L123" s="11"/>
-      <c r="M123" s="11"/>
-      <c r="N123" s="11"/>
-      <c r="O123" s="11"/>
-      <c r="P123" s="11"/>
-      <c r="Q123" s="11"/>
-      <c r="R123" s="11"/>
-      <c r="S123" s="11"/>
       <c r="T123" s="5"/>
     </row>
     <row r="124" spans="2:20">
       <c r="B124" s="4"/>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
-      <c r="F124" s="11"/>
-      <c r="G124" s="11"/>
-      <c r="H124" s="11"/>
-      <c r="I124" s="11"/>
-      <c r="J124" s="11"/>
-      <c r="K124" s="11"/>
-      <c r="L124" s="11"/>
-      <c r="M124" s="11"/>
-      <c r="N124" s="11"/>
-      <c r="O124" s="11"/>
-      <c r="P124" s="11"/>
-      <c r="Q124" s="11"/>
-      <c r="R124" s="11"/>
-      <c r="S124" s="11"/>
       <c r="T124" s="5"/>
     </row>
     <row r="125" spans="2:20">
       <c r="B125" s="4"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
-      <c r="F125" s="11"/>
-      <c r="G125" s="11"/>
-      <c r="H125" s="11"/>
-      <c r="I125" s="11"/>
-      <c r="J125" s="11"/>
-      <c r="K125" s="11"/>
-      <c r="L125" s="11"/>
-      <c r="M125" s="11"/>
-      <c r="N125" s="11"/>
-      <c r="O125" s="11"/>
-      <c r="P125" s="11"/>
-      <c r="Q125" s="11"/>
-      <c r="R125" s="11"/>
-      <c r="S125" s="11"/>
       <c r="T125" s="5"/>
     </row>
     <row r="126" spans="2:20">
       <c r="B126" s="4"/>
-      <c r="C126" s="11"/>
-      <c r="D126" s="11"/>
-      <c r="E126" s="11"/>
-      <c r="F126" s="11"/>
-      <c r="G126" s="11"/>
-      <c r="H126" s="11"/>
-      <c r="I126" s="11"/>
-      <c r="J126" s="11"/>
-      <c r="K126" s="11"/>
-      <c r="L126" s="11"/>
-      <c r="M126" s="11"/>
-      <c r="N126" s="11"/>
-      <c r="O126" s="11"/>
-      <c r="P126" s="11"/>
-      <c r="Q126" s="11"/>
-      <c r="R126" s="11"/>
-      <c r="S126" s="11"/>
       <c r="T126" s="5"/>
     </row>
     <row r="127" spans="2:20">
       <c r="B127" s="4"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11"/>
-      <c r="F127" s="11"/>
-      <c r="G127" s="11"/>
-      <c r="H127" s="11"/>
-      <c r="I127" s="11"/>
-      <c r="J127" s="11"/>
-      <c r="K127" s="11"/>
-      <c r="L127" s="11"/>
-      <c r="M127" s="11"/>
-      <c r="N127" s="11"/>
-      <c r="O127" s="11"/>
-      <c r="P127" s="11"/>
-      <c r="Q127" s="11"/>
-      <c r="R127" s="11"/>
-      <c r="S127" s="11"/>
       <c r="T127" s="5"/>
     </row>
     <row r="128" spans="2:20">
       <c r="B128" s="4"/>
-      <c r="C128" s="11"/>
-      <c r="D128" s="11"/>
-      <c r="E128" s="11"/>
-      <c r="F128" s="11"/>
-      <c r="G128" s="11"/>
-      <c r="H128" s="11"/>
-      <c r="I128" s="11"/>
-      <c r="J128" s="11"/>
-      <c r="K128" s="11"/>
-      <c r="L128" s="11"/>
-      <c r="M128" s="11"/>
-      <c r="N128" s="11"/>
-      <c r="O128" s="11"/>
-      <c r="P128" s="11"/>
-      <c r="Q128" s="11"/>
-      <c r="R128" s="11"/>
-      <c r="S128" s="11"/>
       <c r="T128" s="5"/>
     </row>
     <row r="129" spans="2:20">
       <c r="B129" s="4"/>
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
-      <c r="E129" s="11"/>
-      <c r="F129" s="11"/>
-      <c r="G129" s="11"/>
-      <c r="H129" s="11"/>
-      <c r="I129" s="11"/>
-      <c r="J129" s="11"/>
-      <c r="K129" s="11"/>
-      <c r="L129" s="11"/>
-      <c r="M129" s="11"/>
-      <c r="N129" s="11"/>
-      <c r="O129" s="11"/>
-      <c r="P129" s="11"/>
-      <c r="Q129" s="11"/>
-      <c r="R129" s="11"/>
-      <c r="S129" s="11"/>
       <c r="T129" s="5"/>
     </row>
     <row r="130" spans="2:20">
       <c r="B130" s="4"/>
-      <c r="C130" s="11"/>
-      <c r="D130" s="11"/>
-      <c r="E130" s="11"/>
-      <c r="F130" s="11"/>
-      <c r="G130" s="11"/>
-      <c r="H130" s="11"/>
-      <c r="I130" s="11"/>
-      <c r="J130" s="11"/>
-      <c r="K130" s="11"/>
-      <c r="L130" s="11"/>
-      <c r="M130" s="11"/>
-      <c r="N130" s="11"/>
-      <c r="O130" s="11"/>
-      <c r="P130" s="11"/>
-      <c r="Q130" s="11"/>
-      <c r="R130" s="11"/>
-      <c r="S130" s="11"/>
       <c r="T130" s="5"/>
     </row>
     <row r="131" spans="2:20">
       <c r="B131" s="4"/>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
-      <c r="G131" s="11"/>
-      <c r="H131" s="11"/>
-      <c r="I131" s="11"/>
-      <c r="J131" s="11"/>
-      <c r="K131" s="11"/>
-      <c r="L131" s="11"/>
-      <c r="M131" s="11"/>
-      <c r="N131" s="11"/>
-      <c r="O131" s="11"/>
-      <c r="P131" s="11"/>
-      <c r="Q131" s="11"/>
-      <c r="R131" s="11"/>
-      <c r="S131" s="11"/>
       <c r="T131" s="5"/>
     </row>
     <row r="132" spans="2:20">
@@ -3994,4 +3664,884 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A6E35B-AA98-4C03-8AD6-1F4645D03577}">
+  <dimension ref="B3:P189"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="2:13">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="4"/>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="4"/>
+      <c r="D17" s="6"/>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="9"/>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16">
+      <c r="B46" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="3"/>
+      <c r="O46" t="s">
+        <v>28</v>
+      </c>
+      <c r="P46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16">
+      <c r="B47" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N47" s="5"/>
+      <c r="P47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16">
+      <c r="B48" s="4"/>
+      <c r="N48" s="5"/>
+      <c r="P48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14">
+      <c r="B49" s="4"/>
+      <c r="N49" s="5"/>
+    </row>
+    <row r="50" spans="2:14">
+      <c r="B50" s="4"/>
+      <c r="N50" s="5"/>
+    </row>
+    <row r="51" spans="2:14">
+      <c r="B51" s="4"/>
+      <c r="N51" s="5"/>
+    </row>
+    <row r="52" spans="2:14">
+      <c r="B52" s="4"/>
+      <c r="N52" s="5"/>
+    </row>
+    <row r="53" spans="2:14">
+      <c r="B53" s="4"/>
+      <c r="N53" s="5"/>
+    </row>
+    <row r="54" spans="2:14">
+      <c r="B54" s="4"/>
+      <c r="N54" s="5"/>
+    </row>
+    <row r="55" spans="2:14">
+      <c r="B55" s="4"/>
+      <c r="N55" s="5"/>
+    </row>
+    <row r="56" spans="2:14">
+      <c r="B56" s="4"/>
+      <c r="N56" s="5"/>
+    </row>
+    <row r="57" spans="2:14">
+      <c r="B57" s="4"/>
+      <c r="N57" s="5"/>
+    </row>
+    <row r="58" spans="2:14">
+      <c r="B58" s="4"/>
+      <c r="N58" s="5"/>
+    </row>
+    <row r="59" spans="2:14">
+      <c r="B59" s="4"/>
+      <c r="N59" s="5"/>
+    </row>
+    <row r="60" spans="2:14">
+      <c r="B60" s="7"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="9"/>
+    </row>
+    <row r="63" spans="2:14">
+      <c r="B63" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="3"/>
+    </row>
+    <row r="64" spans="2:14">
+      <c r="B64" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M64" s="5"/>
+    </row>
+    <row r="65" spans="2:13">
+      <c r="B65" s="4"/>
+      <c r="M65" s="5"/>
+    </row>
+    <row r="66" spans="2:13">
+      <c r="B66" s="4"/>
+      <c r="M66" s="5"/>
+    </row>
+    <row r="67" spans="2:13">
+      <c r="B67" s="4"/>
+      <c r="M67" s="5"/>
+    </row>
+    <row r="68" spans="2:13">
+      <c r="B68" s="4"/>
+      <c r="M68" s="5"/>
+    </row>
+    <row r="69" spans="2:13">
+      <c r="B69" s="4"/>
+      <c r="M69" s="5"/>
+    </row>
+    <row r="70" spans="2:13">
+      <c r="B70" s="4"/>
+      <c r="M70" s="5"/>
+    </row>
+    <row r="71" spans="2:13">
+      <c r="B71" s="4"/>
+      <c r="M71" s="5"/>
+    </row>
+    <row r="72" spans="2:13">
+      <c r="B72" s="4"/>
+      <c r="M72" s="5"/>
+    </row>
+    <row r="73" spans="2:13">
+      <c r="B73" s="4"/>
+      <c r="M73" s="5"/>
+    </row>
+    <row r="74" spans="2:13">
+      <c r="B74" s="4"/>
+      <c r="M74" s="5"/>
+    </row>
+    <row r="75" spans="2:13">
+      <c r="B75" s="4"/>
+      <c r="M75" s="5"/>
+    </row>
+    <row r="76" spans="2:13">
+      <c r="B76" s="4"/>
+      <c r="M76" s="5"/>
+    </row>
+    <row r="77" spans="2:13">
+      <c r="B77" s="4"/>
+      <c r="M77" s="5"/>
+    </row>
+    <row r="78" spans="2:13">
+      <c r="B78" s="4"/>
+      <c r="M78" s="5"/>
+    </row>
+    <row r="79" spans="2:13">
+      <c r="B79" s="4"/>
+      <c r="M79" s="5"/>
+    </row>
+    <row r="80" spans="2:13">
+      <c r="B80" s="4"/>
+      <c r="M80" s="5"/>
+    </row>
+    <row r="81" spans="2:13">
+      <c r="B81" s="4"/>
+      <c r="M81" s="5"/>
+    </row>
+    <row r="82" spans="2:13">
+      <c r="B82" s="4"/>
+      <c r="M82" s="5"/>
+    </row>
+    <row r="83" spans="2:13">
+      <c r="B83" s="4"/>
+      <c r="M83" s="5"/>
+    </row>
+    <row r="84" spans="2:13">
+      <c r="B84" s="4"/>
+      <c r="M84" s="5"/>
+    </row>
+    <row r="85" spans="2:13">
+      <c r="B85" s="4"/>
+      <c r="M85" s="5"/>
+    </row>
+    <row r="86" spans="2:13">
+      <c r="B86" s="4"/>
+      <c r="M86" s="5"/>
+    </row>
+    <row r="87" spans="2:13">
+      <c r="B87" s="4"/>
+      <c r="M87" s="5"/>
+    </row>
+    <row r="88" spans="2:13">
+      <c r="B88" s="4"/>
+      <c r="M88" s="5"/>
+    </row>
+    <row r="89" spans="2:13">
+      <c r="B89" s="4"/>
+      <c r="M89" s="5"/>
+    </row>
+    <row r="90" spans="2:13">
+      <c r="B90" s="4"/>
+      <c r="M90" s="5"/>
+    </row>
+    <row r="91" spans="2:13">
+      <c r="B91" s="4"/>
+      <c r="M91" s="5"/>
+    </row>
+    <row r="92" spans="2:13">
+      <c r="B92" s="4"/>
+      <c r="M92" s="5"/>
+    </row>
+    <row r="93" spans="2:13">
+      <c r="B93" s="4"/>
+      <c r="M93" s="5"/>
+    </row>
+    <row r="94" spans="2:13">
+      <c r="B94" s="4"/>
+      <c r="M94" s="5"/>
+    </row>
+    <row r="95" spans="2:13">
+      <c r="B95" s="4"/>
+      <c r="M95" s="5"/>
+    </row>
+    <row r="96" spans="2:13">
+      <c r="B96" s="4"/>
+      <c r="M96" s="5"/>
+    </row>
+    <row r="97" spans="2:15">
+      <c r="B97" s="4"/>
+      <c r="M97" s="5"/>
+    </row>
+    <row r="98" spans="2:15">
+      <c r="B98" s="4"/>
+      <c r="M98" s="5"/>
+    </row>
+    <row r="99" spans="2:15">
+      <c r="B99" s="4"/>
+      <c r="M99" s="5"/>
+    </row>
+    <row r="100" spans="2:15">
+      <c r="B100" s="4"/>
+      <c r="M100" s="5"/>
+    </row>
+    <row r="101" spans="2:15">
+      <c r="B101" s="4"/>
+      <c r="M101" s="5"/>
+    </row>
+    <row r="102" spans="2:15">
+      <c r="B102" s="7"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8"/>
+      <c r="G102" s="8"/>
+      <c r="H102" s="8"/>
+      <c r="I102" s="8"/>
+      <c r="J102" s="8"/>
+      <c r="K102" s="8"/>
+      <c r="L102" s="8"/>
+      <c r="M102" s="9"/>
+    </row>
+    <row r="105" spans="2:15">
+      <c r="B105" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="2"/>
+      <c r="K105" s="2"/>
+      <c r="L105" s="2"/>
+      <c r="M105" s="3"/>
+      <c r="N105" t="s">
+        <v>28</v>
+      </c>
+      <c r="O105" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="106" spans="2:15">
+      <c r="B106" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M106" s="5"/>
+      <c r="O106" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="107" spans="2:15">
+      <c r="B107" s="4"/>
+      <c r="M107" s="5"/>
+    </row>
+    <row r="108" spans="2:15">
+      <c r="B108" s="4"/>
+      <c r="M108" s="5"/>
+    </row>
+    <row r="109" spans="2:15">
+      <c r="B109" s="4"/>
+      <c r="M109" s="5"/>
+    </row>
+    <row r="110" spans="2:15">
+      <c r="B110" s="4"/>
+      <c r="M110" s="5"/>
+    </row>
+    <row r="111" spans="2:15">
+      <c r="B111" s="4"/>
+      <c r="M111" s="5"/>
+    </row>
+    <row r="112" spans="2:15">
+      <c r="B112" s="4"/>
+      <c r="M112" s="5"/>
+    </row>
+    <row r="113" spans="2:13">
+      <c r="B113" s="4"/>
+      <c r="M113" s="5"/>
+    </row>
+    <row r="114" spans="2:13">
+      <c r="B114" s="4"/>
+      <c r="M114" s="5"/>
+    </row>
+    <row r="115" spans="2:13">
+      <c r="B115" s="4"/>
+      <c r="M115" s="5"/>
+    </row>
+    <row r="116" spans="2:13">
+      <c r="B116" s="4"/>
+      <c r="M116" s="5"/>
+    </row>
+    <row r="117" spans="2:13">
+      <c r="B117" s="4"/>
+      <c r="M117" s="5"/>
+    </row>
+    <row r="118" spans="2:13">
+      <c r="B118" s="4"/>
+      <c r="M118" s="5"/>
+    </row>
+    <row r="119" spans="2:13">
+      <c r="B119" s="4"/>
+      <c r="M119" s="5"/>
+    </row>
+    <row r="120" spans="2:13">
+      <c r="B120" s="4"/>
+      <c r="M120" s="5"/>
+    </row>
+    <row r="121" spans="2:13">
+      <c r="B121" s="4"/>
+      <c r="M121" s="5"/>
+    </row>
+    <row r="122" spans="2:13">
+      <c r="B122" s="4"/>
+      <c r="M122" s="5"/>
+    </row>
+    <row r="123" spans="2:13">
+      <c r="B123" s="4"/>
+      <c r="M123" s="5"/>
+    </row>
+    <row r="124" spans="2:13">
+      <c r="B124" s="4"/>
+      <c r="M124" s="5"/>
+    </row>
+    <row r="125" spans="2:13">
+      <c r="B125" s="4"/>
+      <c r="M125" s="5"/>
+    </row>
+    <row r="126" spans="2:13">
+      <c r="B126" s="4"/>
+      <c r="M126" s="5"/>
+    </row>
+    <row r="127" spans="2:13">
+      <c r="B127" s="4"/>
+      <c r="M127" s="5"/>
+    </row>
+    <row r="128" spans="2:13">
+      <c r="B128" s="4"/>
+      <c r="M128" s="5"/>
+    </row>
+    <row r="129" spans="2:13">
+      <c r="B129" s="4"/>
+      <c r="M129" s="5"/>
+    </row>
+    <row r="130" spans="2:13">
+      <c r="B130" s="4"/>
+      <c r="M130" s="5"/>
+    </row>
+    <row r="131" spans="2:13">
+      <c r="B131" s="4"/>
+      <c r="M131" s="5"/>
+    </row>
+    <row r="132" spans="2:13">
+      <c r="B132" s="4"/>
+      <c r="M132" s="5"/>
+    </row>
+    <row r="133" spans="2:13">
+      <c r="B133" s="4"/>
+      <c r="M133" s="5"/>
+    </row>
+    <row r="134" spans="2:13">
+      <c r="B134" s="4"/>
+      <c r="M134" s="5"/>
+    </row>
+    <row r="135" spans="2:13">
+      <c r="B135" s="4"/>
+      <c r="M135" s="5"/>
+    </row>
+    <row r="136" spans="2:13">
+      <c r="B136" s="4"/>
+      <c r="M136" s="5"/>
+    </row>
+    <row r="137" spans="2:13">
+      <c r="B137" s="4"/>
+      <c r="M137" s="5"/>
+    </row>
+    <row r="138" spans="2:13">
+      <c r="B138" s="4"/>
+      <c r="M138" s="5"/>
+    </row>
+    <row r="139" spans="2:13">
+      <c r="B139" s="4"/>
+      <c r="M139" s="5"/>
+    </row>
+    <row r="140" spans="2:13">
+      <c r="B140" s="4"/>
+      <c r="M140" s="5"/>
+    </row>
+    <row r="141" spans="2:13">
+      <c r="B141" s="4"/>
+      <c r="M141" s="5"/>
+    </row>
+    <row r="142" spans="2:13">
+      <c r="B142" s="7"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+      <c r="F142" s="8"/>
+      <c r="G142" s="8"/>
+      <c r="H142" s="8"/>
+      <c r="I142" s="8"/>
+      <c r="J142" s="8"/>
+      <c r="K142" s="8"/>
+      <c r="L142" s="8"/>
+      <c r="M142" s="9"/>
+    </row>
+    <row r="145" spans="2:15">
+      <c r="B145" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+      <c r="J145" s="2"/>
+      <c r="K145" s="2"/>
+      <c r="L145" s="2"/>
+      <c r="M145" s="3"/>
+      <c r="N145" t="s">
+        <v>28</v>
+      </c>
+      <c r="O145" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="146" spans="2:15">
+      <c r="B146" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M146" s="5"/>
+    </row>
+    <row r="147" spans="2:15">
+      <c r="B147" s="4"/>
+      <c r="M147" s="5"/>
+    </row>
+    <row r="148" spans="2:15">
+      <c r="B148" s="4"/>
+      <c r="M148" s="5"/>
+    </row>
+    <row r="149" spans="2:15">
+      <c r="B149" s="4"/>
+      <c r="M149" s="5"/>
+    </row>
+    <row r="150" spans="2:15">
+      <c r="B150" s="4"/>
+      <c r="M150" s="5"/>
+    </row>
+    <row r="151" spans="2:15">
+      <c r="B151" s="4"/>
+      <c r="M151" s="5"/>
+    </row>
+    <row r="152" spans="2:15">
+      <c r="B152" s="4"/>
+      <c r="M152" s="5"/>
+    </row>
+    <row r="153" spans="2:15">
+      <c r="B153" s="4"/>
+      <c r="M153" s="5"/>
+    </row>
+    <row r="154" spans="2:15">
+      <c r="B154" s="4"/>
+      <c r="M154" s="5"/>
+    </row>
+    <row r="155" spans="2:15">
+      <c r="B155" s="4"/>
+      <c r="M155" s="5"/>
+    </row>
+    <row r="156" spans="2:15">
+      <c r="B156" s="4"/>
+      <c r="M156" s="5"/>
+    </row>
+    <row r="157" spans="2:15">
+      <c r="B157" s="7"/>
+      <c r="C157" s="8"/>
+      <c r="D157" s="8"/>
+      <c r="E157" s="8"/>
+      <c r="F157" s="8"/>
+      <c r="G157" s="8"/>
+      <c r="H157" s="8"/>
+      <c r="I157" s="8"/>
+      <c r="J157" s="8"/>
+      <c r="K157" s="8"/>
+      <c r="L157" s="8"/>
+      <c r="M157" s="9"/>
+    </row>
+    <row r="160" spans="2:15">
+      <c r="B160" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
+      <c r="J160" s="2"/>
+      <c r="K160" s="2"/>
+      <c r="L160" s="2"/>
+      <c r="M160" s="3"/>
+      <c r="N160" t="s">
+        <v>28</v>
+      </c>
+      <c r="O160" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="161" spans="2:15">
+      <c r="B161" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M161" s="5"/>
+    </row>
+    <row r="162" spans="2:15">
+      <c r="B162" s="4"/>
+      <c r="M162" s="5"/>
+    </row>
+    <row r="163" spans="2:15">
+      <c r="B163" s="4"/>
+      <c r="M163" s="5"/>
+    </row>
+    <row r="164" spans="2:15">
+      <c r="B164" s="4"/>
+      <c r="M164" s="5"/>
+    </row>
+    <row r="165" spans="2:15">
+      <c r="B165" s="4"/>
+      <c r="M165" s="5"/>
+    </row>
+    <row r="166" spans="2:15">
+      <c r="B166" s="4"/>
+      <c r="M166" s="5"/>
+    </row>
+    <row r="167" spans="2:15">
+      <c r="B167" s="4"/>
+      <c r="M167" s="5"/>
+    </row>
+    <row r="168" spans="2:15">
+      <c r="B168" s="4"/>
+      <c r="M168" s="5"/>
+    </row>
+    <row r="169" spans="2:15">
+      <c r="B169" s="4"/>
+      <c r="M169" s="5"/>
+    </row>
+    <row r="170" spans="2:15">
+      <c r="B170" s="4"/>
+      <c r="M170" s="5"/>
+    </row>
+    <row r="171" spans="2:15">
+      <c r="B171" s="4"/>
+      <c r="M171" s="5"/>
+    </row>
+    <row r="172" spans="2:15">
+      <c r="B172" s="4"/>
+      <c r="M172" s="5"/>
+    </row>
+    <row r="173" spans="2:15">
+      <c r="B173" s="7"/>
+      <c r="C173" s="8"/>
+      <c r="D173" s="8"/>
+      <c r="E173" s="8"/>
+      <c r="F173" s="8"/>
+      <c r="G173" s="8"/>
+      <c r="H173" s="8"/>
+      <c r="I173" s="8"/>
+      <c r="J173" s="8"/>
+      <c r="K173" s="8"/>
+      <c r="L173" s="8"/>
+      <c r="M173" s="9"/>
+    </row>
+    <row r="176" spans="2:15">
+      <c r="B176" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C176" s="2"/>
+      <c r="D176" s="2"/>
+      <c r="E176" s="2"/>
+      <c r="F176" s="2"/>
+      <c r="G176" s="2"/>
+      <c r="H176" s="2"/>
+      <c r="I176" s="2"/>
+      <c r="J176" s="2"/>
+      <c r="K176" s="2"/>
+      <c r="L176" s="2"/>
+      <c r="M176" s="3"/>
+      <c r="N176" t="s">
+        <v>28</v>
+      </c>
+      <c r="O176" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="177" spans="2:13">
+      <c r="B177" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M177" s="5"/>
+    </row>
+    <row r="178" spans="2:13">
+      <c r="B178" s="4"/>
+      <c r="M178" s="5"/>
+    </row>
+    <row r="179" spans="2:13">
+      <c r="B179" s="4"/>
+      <c r="M179" s="5"/>
+    </row>
+    <row r="180" spans="2:13">
+      <c r="B180" s="4"/>
+      <c r="M180" s="5"/>
+    </row>
+    <row r="181" spans="2:13">
+      <c r="B181" s="4"/>
+      <c r="M181" s="5"/>
+    </row>
+    <row r="182" spans="2:13">
+      <c r="B182" s="4"/>
+      <c r="M182" s="5"/>
+    </row>
+    <row r="183" spans="2:13">
+      <c r="B183" s="4"/>
+      <c r="M183" s="5"/>
+    </row>
+    <row r="184" spans="2:13">
+      <c r="B184" s="4"/>
+      <c r="M184" s="5"/>
+    </row>
+    <row r="185" spans="2:13">
+      <c r="B185" s="4"/>
+      <c r="M185" s="5"/>
+    </row>
+    <row r="186" spans="2:13">
+      <c r="B186" s="4"/>
+      <c r="M186" s="5"/>
+    </row>
+    <row r="187" spans="2:13">
+      <c r="B187" s="4"/>
+      <c r="M187" s="5"/>
+    </row>
+    <row r="188" spans="2:13">
+      <c r="B188" s="4"/>
+      <c r="M188" s="5"/>
+    </row>
+    <row r="189" spans="2:13">
+      <c r="B189" s="7"/>
+      <c r="C189" s="8"/>
+      <c r="D189" s="8"/>
+      <c r="E189" s="8"/>
+      <c r="F189" s="8"/>
+      <c r="G189" s="8"/>
+      <c r="H189" s="8"/>
+      <c r="I189" s="8"/>
+      <c r="J189" s="8"/>
+      <c r="K189" s="8"/>
+      <c r="L189" s="8"/>
+      <c r="M189" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Inner Join & Join with the ON Clause
</commit_message>
<xml_diff>
--- a/11.Joining-Multiple-Tables/Joining-Multiple-Tables.xlsx
+++ b/11.Joining-Multiple-Tables/Joining-Multiple-Tables.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\oracle\11.Joining-Multiple-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE960B2C-9AE9-4FB9-BADE-0BFD0959D5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC04EE0-EBCC-477B-B896-25FB6244A971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29130" yWindow="180" windowWidth="25530" windowHeight="13155" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29130" yWindow="180" windowWidth="25530" windowHeight="13155" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oracle SQL Join Types" sheetId="1" r:id="rId1"/>
     <sheet name="Natural Join" sheetId="2" r:id="rId2"/>
     <sheet name="Join with the USING Clause" sheetId="3" r:id="rId3"/>
     <sheet name="Handling Ambiguous Column Names" sheetId="4" r:id="rId4"/>
+    <sheet name="InnerJoin&amp;JoinWithTheONClause" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
   <si>
     <t>oracle</t>
     <phoneticPr fontId="1"/>
@@ -798,12 +799,358 @@
     </r>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>3.Handling+Ambiguous+Column+Names+(Code+Samples).sql</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4.Inner+Join+&amp;+Join+with+the+ON+Clause+(Code+Samples).sql</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT e.first_name, e.last_name, d.manager_id, d.department_name </t>
+  </si>
+  <si>
+    <t>FROM employees e JOIN departments d</t>
+  </si>
+  <si>
+    <t>ON(e.department_id = d.department_id AND e.manager_id = d.manager_id);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FROM employees e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JOIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> departments d</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FROM employees e </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INNER JOIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> departments d</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT e.first_name, e.last_name, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>manager_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, d.department_name </t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>USING(department_id,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> manager_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">we use columns with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>USING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> clause we can not give aliases to those columns</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT e.first_name, e.last_name, d.manager_id, d.department_name </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>ON and USING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> both of them</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> allow us to join unlimited tables. The differences is that the USING clause requires the</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">join columns to have </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>exactly the same name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. But the ON clause also works when the join columns have </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>difference names</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(e.department_id = d.department_id AND </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e.employee_id = d.manager_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Basically a join that returns only the rows which satisfy the join condition is considered as an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inner join</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. It can be created by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>USING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> clause, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> clause or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Yu Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NATURAL JOIN </t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -828,6 +1175,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="3"/>
       <charset val="128"/>
@@ -934,7 +1289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -945,6 +1300,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1889,6 +2247,351 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447529</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3D86CF6-D5E1-C095-0352-C3BF26C6E8C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781049" y="4733925"/>
+          <a:ext cx="10185255" cy="4457700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>88551</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A66754CB-6D6E-365E-C44E-7EA16514C7A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="815975" y="10401300"/>
+          <a:ext cx="5918200" cy="7521226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>282575</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矢印: 上下 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{325606C8-CC66-4A77-601D-F626E74BDF54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3333750" y="18294350"/>
+          <a:ext cx="234950" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>130175</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>75938</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="図 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05BEEE90-99B6-A884-2E18-1DA9272B2D3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="828675" y="19754850"/>
+          <a:ext cx="5873750" cy="7753088"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>155025</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="図 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E26C954-36F2-1A72-FA6E-B0B88FE634AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="29298901"/>
+          <a:ext cx="5984325" cy="8267700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>168275</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="矢印: 上下 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E928B05-E614-4CC4-AC3A-2756140B01EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3219450" y="27917775"/>
+          <a:ext cx="234950" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="upDownArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>82549</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>44449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>75330</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="図 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A0A8274-9DE0-8A52-BDF7-6898DEA284A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="739774" y="38906449"/>
+          <a:ext cx="6022975" cy="4374281"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3670,8 +4373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A6E35B-AA98-4C03-8AD6-1F4645D03577}">
   <dimension ref="B3:P189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -3786,7 +4489,9 @@
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="4"/>
-      <c r="D17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="2:13">
@@ -4544,4 +5249,1882 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7E6A0E-FB1A-4AD9-B4ED-365961D1038D}">
+  <dimension ref="B3:M192"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="2:13">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="2:13">
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="2:13">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="2:13">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="2:13">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="2:13">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="2:13">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="B13" s="4"/>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="4"/>
+      <c r="D17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="4"/>
+      <c r="D18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M18" s="5"/>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="B21" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="5"/>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="B48" s="4"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="2:11">
+      <c r="B49" s="4"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="2:11">
+      <c r="B50" s="4"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="2:11">
+      <c r="B51" s="4"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="5"/>
+    </row>
+    <row r="52" spans="2:11">
+      <c r="B52" s="4"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="5"/>
+    </row>
+    <row r="53" spans="2:11">
+      <c r="B53" s="4"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="5"/>
+    </row>
+    <row r="54" spans="2:11">
+      <c r="B54" s="4"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="5"/>
+    </row>
+    <row r="55" spans="2:11">
+      <c r="B55" s="4"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="5"/>
+    </row>
+    <row r="56" spans="2:11">
+      <c r="B56" s="4"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="5"/>
+    </row>
+    <row r="57" spans="2:11">
+      <c r="B57" s="4"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="5"/>
+    </row>
+    <row r="58" spans="2:11">
+      <c r="B58" s="4"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="5"/>
+    </row>
+    <row r="59" spans="2:11">
+      <c r="B59" s="4"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="5"/>
+    </row>
+    <row r="60" spans="2:11">
+      <c r="B60" s="4"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="5"/>
+    </row>
+    <row r="61" spans="2:11">
+      <c r="B61" s="4"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="5"/>
+    </row>
+    <row r="62" spans="2:11">
+      <c r="B62" s="4"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="5"/>
+    </row>
+    <row r="63" spans="2:11">
+      <c r="B63" s="4"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="5"/>
+    </row>
+    <row r="64" spans="2:11">
+      <c r="B64" s="4"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="5"/>
+    </row>
+    <row r="65" spans="2:11">
+      <c r="B65" s="4"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="K65" s="5"/>
+    </row>
+    <row r="66" spans="2:11">
+      <c r="B66" s="4"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="5"/>
+    </row>
+    <row r="67" spans="2:11">
+      <c r="B67" s="4"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="11"/>
+      <c r="K67" s="5"/>
+    </row>
+    <row r="68" spans="2:11">
+      <c r="B68" s="4"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="11"/>
+      <c r="K68" s="5"/>
+    </row>
+    <row r="69" spans="2:11">
+      <c r="B69" s="4"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="5"/>
+    </row>
+    <row r="70" spans="2:11">
+      <c r="B70" s="4"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="5"/>
+    </row>
+    <row r="71" spans="2:11">
+      <c r="B71" s="4"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="5"/>
+    </row>
+    <row r="72" spans="2:11">
+      <c r="B72" s="4"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="11"/>
+      <c r="K72" s="5"/>
+    </row>
+    <row r="73" spans="2:11">
+      <c r="B73" s="4"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="11"/>
+      <c r="K73" s="5"/>
+    </row>
+    <row r="74" spans="2:11">
+      <c r="B74" s="4"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="11"/>
+      <c r="J74" s="11"/>
+      <c r="K74" s="5"/>
+    </row>
+    <row r="75" spans="2:11">
+      <c r="B75" s="4"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="11"/>
+      <c r="K75" s="5"/>
+    </row>
+    <row r="76" spans="2:11">
+      <c r="B76" s="4"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="11"/>
+      <c r="K76" s="5"/>
+    </row>
+    <row r="77" spans="2:11">
+      <c r="B77" s="4"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="11"/>
+      <c r="K77" s="5"/>
+    </row>
+    <row r="78" spans="2:11">
+      <c r="B78" s="4"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="5"/>
+    </row>
+    <row r="79" spans="2:11">
+      <c r="B79" s="4"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="11"/>
+      <c r="K79" s="5"/>
+    </row>
+    <row r="80" spans="2:11">
+      <c r="B80" s="4"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="11"/>
+      <c r="K80" s="5"/>
+    </row>
+    <row r="81" spans="2:11">
+      <c r="B81" s="7"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="8"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8"/>
+      <c r="K81" s="9"/>
+    </row>
+    <row r="86" spans="2:11">
+      <c r="B86" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="3"/>
+    </row>
+    <row r="87" spans="2:11">
+      <c r="B87" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="11"/>
+      <c r="K87" s="5"/>
+    </row>
+    <row r="88" spans="2:11">
+      <c r="B88" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="11"/>
+      <c r="K88" s="5"/>
+    </row>
+    <row r="89" spans="2:11">
+      <c r="B89" s="4"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="11"/>
+      <c r="K89" s="5"/>
+    </row>
+    <row r="90" spans="2:11">
+      <c r="B90" s="4"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="11"/>
+      <c r="I90" s="11"/>
+      <c r="J90" s="11"/>
+      <c r="K90" s="5"/>
+    </row>
+    <row r="91" spans="2:11">
+      <c r="B91" s="4"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="11"/>
+      <c r="I91" s="11"/>
+      <c r="J91" s="11"/>
+      <c r="K91" s="5"/>
+    </row>
+    <row r="92" spans="2:11">
+      <c r="B92" s="4"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="11"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="5"/>
+    </row>
+    <row r="93" spans="2:11">
+      <c r="B93" s="4"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="11"/>
+      <c r="J93" s="11"/>
+      <c r="K93" s="5"/>
+    </row>
+    <row r="94" spans="2:11">
+      <c r="B94" s="4"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="11"/>
+      <c r="I94" s="11"/>
+      <c r="J94" s="11"/>
+      <c r="K94" s="5"/>
+    </row>
+    <row r="95" spans="2:11">
+      <c r="B95" s="4"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="11"/>
+      <c r="I95" s="11"/>
+      <c r="J95" s="11"/>
+      <c r="K95" s="5"/>
+    </row>
+    <row r="96" spans="2:11">
+      <c r="B96" s="4"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="11"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="11"/>
+      <c r="J96" s="11"/>
+      <c r="K96" s="5"/>
+    </row>
+    <row r="97" spans="2:11">
+      <c r="B97" s="4"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="11"/>
+      <c r="I97" s="11"/>
+      <c r="J97" s="11"/>
+      <c r="K97" s="5"/>
+    </row>
+    <row r="98" spans="2:11">
+      <c r="B98" s="4"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+      <c r="G98" s="11"/>
+      <c r="H98" s="11"/>
+      <c r="I98" s="11"/>
+      <c r="J98" s="11"/>
+      <c r="K98" s="5"/>
+    </row>
+    <row r="99" spans="2:11">
+      <c r="B99" s="4"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="11"/>
+      <c r="H99" s="11"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="11"/>
+      <c r="K99" s="5"/>
+    </row>
+    <row r="100" spans="2:11">
+      <c r="B100" s="4"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+      <c r="H100" s="11"/>
+      <c r="I100" s="11"/>
+      <c r="J100" s="11"/>
+      <c r="K100" s="5"/>
+    </row>
+    <row r="101" spans="2:11">
+      <c r="B101" s="4"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="11"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11"/>
+      <c r="G101" s="11"/>
+      <c r="H101" s="11"/>
+      <c r="I101" s="11"/>
+      <c r="J101" s="11"/>
+      <c r="K101" s="5"/>
+    </row>
+    <row r="102" spans="2:11">
+      <c r="B102" s="4"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11"/>
+      <c r="E102" s="11"/>
+      <c r="F102" s="11"/>
+      <c r="G102" s="11"/>
+      <c r="H102" s="11"/>
+      <c r="I102" s="11"/>
+      <c r="J102" s="11"/>
+      <c r="K102" s="5"/>
+    </row>
+    <row r="103" spans="2:11">
+      <c r="B103" s="4"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="11"/>
+      <c r="G103" s="11"/>
+      <c r="H103" s="11"/>
+      <c r="I103" s="11"/>
+      <c r="J103" s="11"/>
+      <c r="K103" s="5"/>
+    </row>
+    <row r="104" spans="2:11">
+      <c r="B104" s="4"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="11"/>
+      <c r="G104" s="11"/>
+      <c r="H104" s="11"/>
+      <c r="I104" s="11"/>
+      <c r="J104" s="11"/>
+      <c r="K104" s="5"/>
+    </row>
+    <row r="105" spans="2:11">
+      <c r="B105" s="4"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
+      <c r="G105" s="11"/>
+      <c r="H105" s="11"/>
+      <c r="I105" s="11"/>
+      <c r="J105" s="11"/>
+      <c r="K105" s="5"/>
+    </row>
+    <row r="106" spans="2:11">
+      <c r="B106" s="4"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
+      <c r="G106" s="11"/>
+      <c r="H106" s="11"/>
+      <c r="I106" s="11"/>
+      <c r="J106" s="11"/>
+      <c r="K106" s="5"/>
+    </row>
+    <row r="107" spans="2:11">
+      <c r="B107" s="4"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="11"/>
+      <c r="H107" s="11"/>
+      <c r="I107" s="11"/>
+      <c r="J107" s="11"/>
+      <c r="K107" s="5"/>
+    </row>
+    <row r="108" spans="2:11">
+      <c r="B108" s="4"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="11"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="11"/>
+      <c r="K108" s="5"/>
+    </row>
+    <row r="109" spans="2:11">
+      <c r="B109" s="4"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
+      <c r="G109" s="11"/>
+      <c r="H109" s="11"/>
+      <c r="I109" s="11"/>
+      <c r="J109" s="11"/>
+      <c r="K109" s="5"/>
+    </row>
+    <row r="110" spans="2:11">
+      <c r="B110" s="4"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="11"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="11"/>
+      <c r="I110" s="11"/>
+      <c r="J110" s="11"/>
+      <c r="K110" s="5"/>
+    </row>
+    <row r="111" spans="2:11">
+      <c r="B111" s="4"/>
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="11"/>
+      <c r="G111" s="11"/>
+      <c r="H111" s="11"/>
+      <c r="I111" s="11"/>
+      <c r="J111" s="11"/>
+      <c r="K111" s="5"/>
+    </row>
+    <row r="112" spans="2:11">
+      <c r="B112" s="4"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
+      <c r="G112" s="11"/>
+      <c r="H112" s="11"/>
+      <c r="I112" s="11"/>
+      <c r="J112" s="11"/>
+      <c r="K112" s="5"/>
+    </row>
+    <row r="113" spans="2:13">
+      <c r="B113" s="4"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="11"/>
+      <c r="F113" s="11"/>
+      <c r="G113" s="11"/>
+      <c r="H113" s="11"/>
+      <c r="I113" s="11"/>
+      <c r="J113" s="11"/>
+      <c r="K113" s="5"/>
+    </row>
+    <row r="114" spans="2:13">
+      <c r="B114" s="4"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
+      <c r="G114" s="11"/>
+      <c r="H114" s="11"/>
+      <c r="I114" s="11"/>
+      <c r="J114" s="11"/>
+      <c r="K114" s="5"/>
+    </row>
+    <row r="115" spans="2:13">
+      <c r="B115" s="4"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="11"/>
+      <c r="F115" s="11"/>
+      <c r="G115" s="11"/>
+      <c r="H115" s="11"/>
+      <c r="I115" s="11"/>
+      <c r="J115" s="11"/>
+      <c r="K115" s="5"/>
+    </row>
+    <row r="116" spans="2:13">
+      <c r="B116" s="4"/>
+      <c r="C116" s="11"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="11"/>
+      <c r="F116" s="11"/>
+      <c r="G116" s="11"/>
+      <c r="H116" s="11"/>
+      <c r="I116" s="11"/>
+      <c r="J116" s="11"/>
+      <c r="K116" s="5"/>
+    </row>
+    <row r="117" spans="2:13">
+      <c r="B117" s="4"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="11"/>
+      <c r="F117" s="11"/>
+      <c r="G117" s="11"/>
+      <c r="H117" s="11"/>
+      <c r="I117" s="11"/>
+      <c r="J117" s="11"/>
+      <c r="K117" s="5"/>
+    </row>
+    <row r="118" spans="2:13">
+      <c r="B118" s="4"/>
+      <c r="C118" s="11"/>
+      <c r="D118" s="11"/>
+      <c r="E118" s="11"/>
+      <c r="F118" s="11"/>
+      <c r="G118" s="11"/>
+      <c r="H118" s="11"/>
+      <c r="I118" s="11"/>
+      <c r="J118" s="11"/>
+      <c r="K118" s="5"/>
+    </row>
+    <row r="119" spans="2:13">
+      <c r="B119" s="4"/>
+      <c r="C119" s="11"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="11"/>
+      <c r="F119" s="11"/>
+      <c r="G119" s="11"/>
+      <c r="H119" s="11"/>
+      <c r="I119" s="11"/>
+      <c r="J119" s="11"/>
+      <c r="K119" s="5"/>
+    </row>
+    <row r="120" spans="2:13">
+      <c r="B120" s="4"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="11"/>
+      <c r="E120" s="11"/>
+      <c r="F120" s="11"/>
+      <c r="G120" s="11"/>
+      <c r="H120" s="11"/>
+      <c r="I120" s="11"/>
+      <c r="J120" s="11"/>
+      <c r="K120" s="5"/>
+    </row>
+    <row r="121" spans="2:13">
+      <c r="B121" s="4"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11"/>
+      <c r="G121" s="11"/>
+      <c r="H121" s="11"/>
+      <c r="I121" s="11"/>
+      <c r="J121" s="11"/>
+      <c r="K121" s="5"/>
+    </row>
+    <row r="122" spans="2:13">
+      <c r="B122" s="4"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="11"/>
+      <c r="F122" s="11"/>
+      <c r="G122" s="11"/>
+      <c r="H122" s="11"/>
+      <c r="I122" s="11"/>
+      <c r="J122" s="11"/>
+      <c r="K122" s="5"/>
+    </row>
+    <row r="123" spans="2:13">
+      <c r="B123" s="7"/>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
+      <c r="F123" s="8"/>
+      <c r="G123" s="8"/>
+      <c r="H123" s="8"/>
+      <c r="I123" s="8"/>
+      <c r="J123" s="8"/>
+      <c r="K123" s="9"/>
+    </row>
+    <row r="128" spans="2:13">
+      <c r="B128" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+      <c r="J128" s="2"/>
+      <c r="K128" s="3"/>
+      <c r="L128" t="s">
+        <v>28</v>
+      </c>
+      <c r="M128" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="129" spans="2:11">
+      <c r="B129" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
+      <c r="E129" s="11"/>
+      <c r="F129" s="11"/>
+      <c r="G129" s="11"/>
+      <c r="H129" s="11"/>
+      <c r="I129" s="11"/>
+      <c r="J129" s="11"/>
+      <c r="K129" s="5"/>
+    </row>
+    <row r="130" spans="2:11">
+      <c r="B130" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C130" s="11"/>
+      <c r="D130" s="11"/>
+      <c r="E130" s="11"/>
+      <c r="F130" s="11"/>
+      <c r="G130" s="11"/>
+      <c r="H130" s="11"/>
+      <c r="I130" s="11"/>
+      <c r="J130" s="11"/>
+      <c r="K130" s="5"/>
+    </row>
+    <row r="131" spans="2:11">
+      <c r="B131" s="4"/>
+      <c r="C131" s="11"/>
+      <c r="D131" s="11"/>
+      <c r="E131" s="11"/>
+      <c r="F131" s="11"/>
+      <c r="G131" s="11"/>
+      <c r="H131" s="11"/>
+      <c r="I131" s="11"/>
+      <c r="J131" s="11"/>
+      <c r="K131" s="5"/>
+    </row>
+    <row r="132" spans="2:11">
+      <c r="B132" s="4"/>
+      <c r="C132" s="11"/>
+      <c r="D132" s="11"/>
+      <c r="E132" s="11"/>
+      <c r="F132" s="11"/>
+      <c r="G132" s="11"/>
+      <c r="H132" s="11"/>
+      <c r="I132" s="11"/>
+      <c r="J132" s="11"/>
+      <c r="K132" s="5"/>
+    </row>
+    <row r="133" spans="2:11">
+      <c r="B133" s="4"/>
+      <c r="C133" s="11"/>
+      <c r="D133" s="11"/>
+      <c r="E133" s="11"/>
+      <c r="F133" s="11"/>
+      <c r="G133" s="11"/>
+      <c r="H133" s="11"/>
+      <c r="I133" s="11"/>
+      <c r="J133" s="11"/>
+      <c r="K133" s="5"/>
+    </row>
+    <row r="134" spans="2:11">
+      <c r="B134" s="4"/>
+      <c r="C134" s="11"/>
+      <c r="D134" s="11"/>
+      <c r="E134" s="11"/>
+      <c r="F134" s="11"/>
+      <c r="G134" s="11"/>
+      <c r="H134" s="11"/>
+      <c r="I134" s="11"/>
+      <c r="J134" s="11"/>
+      <c r="K134" s="5"/>
+    </row>
+    <row r="135" spans="2:11">
+      <c r="B135" s="4"/>
+      <c r="C135" s="11"/>
+      <c r="D135" s="11"/>
+      <c r="E135" s="11"/>
+      <c r="F135" s="11"/>
+      <c r="G135" s="11"/>
+      <c r="H135" s="11"/>
+      <c r="I135" s="11"/>
+      <c r="J135" s="11"/>
+      <c r="K135" s="5"/>
+    </row>
+    <row r="136" spans="2:11">
+      <c r="B136" s="4"/>
+      <c r="C136" s="11"/>
+      <c r="D136" s="11"/>
+      <c r="E136" s="11"/>
+      <c r="F136" s="11"/>
+      <c r="G136" s="11"/>
+      <c r="H136" s="11"/>
+      <c r="I136" s="11"/>
+      <c r="J136" s="11"/>
+      <c r="K136" s="5"/>
+    </row>
+    <row r="137" spans="2:11">
+      <c r="B137" s="4"/>
+      <c r="C137" s="11"/>
+      <c r="D137" s="11"/>
+      <c r="E137" s="11"/>
+      <c r="F137" s="11"/>
+      <c r="G137" s="11"/>
+      <c r="H137" s="11"/>
+      <c r="I137" s="11"/>
+      <c r="J137" s="11"/>
+      <c r="K137" s="5"/>
+    </row>
+    <row r="138" spans="2:11">
+      <c r="B138" s="4"/>
+      <c r="C138" s="11"/>
+      <c r="D138" s="11"/>
+      <c r="E138" s="11"/>
+      <c r="F138" s="11"/>
+      <c r="G138" s="11"/>
+      <c r="H138" s="11"/>
+      <c r="I138" s="11"/>
+      <c r="J138" s="11"/>
+      <c r="K138" s="5"/>
+    </row>
+    <row r="139" spans="2:11">
+      <c r="B139" s="4"/>
+      <c r="C139" s="11"/>
+      <c r="D139" s="11"/>
+      <c r="E139" s="11"/>
+      <c r="F139" s="11"/>
+      <c r="G139" s="11"/>
+      <c r="H139" s="11"/>
+      <c r="I139" s="11"/>
+      <c r="J139" s="11"/>
+      <c r="K139" s="5"/>
+    </row>
+    <row r="140" spans="2:11">
+      <c r="B140" s="4"/>
+      <c r="C140" s="11"/>
+      <c r="D140" s="11"/>
+      <c r="E140" s="11"/>
+      <c r="F140" s="11"/>
+      <c r="G140" s="11"/>
+      <c r="H140" s="11"/>
+      <c r="I140" s="11"/>
+      <c r="J140" s="11"/>
+      <c r="K140" s="5"/>
+    </row>
+    <row r="141" spans="2:11">
+      <c r="B141" s="4"/>
+      <c r="C141" s="11"/>
+      <c r="D141" s="11"/>
+      <c r="E141" s="11"/>
+      <c r="F141" s="11"/>
+      <c r="G141" s="11"/>
+      <c r="H141" s="11"/>
+      <c r="I141" s="11"/>
+      <c r="J141" s="11"/>
+      <c r="K141" s="5"/>
+    </row>
+    <row r="142" spans="2:11">
+      <c r="B142" s="4"/>
+      <c r="C142" s="11"/>
+      <c r="D142" s="11"/>
+      <c r="E142" s="11"/>
+      <c r="F142" s="11"/>
+      <c r="G142" s="11"/>
+      <c r="H142" s="11"/>
+      <c r="I142" s="11"/>
+      <c r="J142" s="11"/>
+      <c r="K142" s="5"/>
+    </row>
+    <row r="143" spans="2:11">
+      <c r="B143" s="4"/>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
+      <c r="E143" s="11"/>
+      <c r="F143" s="11"/>
+      <c r="G143" s="11"/>
+      <c r="H143" s="11"/>
+      <c r="I143" s="11"/>
+      <c r="J143" s="11"/>
+      <c r="K143" s="5"/>
+    </row>
+    <row r="144" spans="2:11">
+      <c r="B144" s="4"/>
+      <c r="C144" s="11"/>
+      <c r="D144" s="11"/>
+      <c r="E144" s="11"/>
+      <c r="F144" s="11"/>
+      <c r="G144" s="11"/>
+      <c r="H144" s="11"/>
+      <c r="I144" s="11"/>
+      <c r="J144" s="11"/>
+      <c r="K144" s="5"/>
+    </row>
+    <row r="145" spans="2:11">
+      <c r="B145" s="4"/>
+      <c r="C145" s="11"/>
+      <c r="D145" s="11"/>
+      <c r="E145" s="11"/>
+      <c r="F145" s="11"/>
+      <c r="G145" s="11"/>
+      <c r="H145" s="11"/>
+      <c r="I145" s="11"/>
+      <c r="J145" s="11"/>
+      <c r="K145" s="5"/>
+    </row>
+    <row r="146" spans="2:11">
+      <c r="B146" s="4"/>
+      <c r="C146" s="11"/>
+      <c r="D146" s="11"/>
+      <c r="E146" s="11"/>
+      <c r="F146" s="11"/>
+      <c r="G146" s="11"/>
+      <c r="H146" s="11"/>
+      <c r="I146" s="11"/>
+      <c r="J146" s="11"/>
+      <c r="K146" s="5"/>
+    </row>
+    <row r="147" spans="2:11">
+      <c r="B147" s="4"/>
+      <c r="C147" s="11"/>
+      <c r="D147" s="11"/>
+      <c r="E147" s="11"/>
+      <c r="F147" s="11"/>
+      <c r="G147" s="11"/>
+      <c r="H147" s="11"/>
+      <c r="I147" s="11"/>
+      <c r="J147" s="11"/>
+      <c r="K147" s="5"/>
+    </row>
+    <row r="148" spans="2:11">
+      <c r="B148" s="4"/>
+      <c r="C148" s="11"/>
+      <c r="D148" s="11"/>
+      <c r="E148" s="11"/>
+      <c r="F148" s="11"/>
+      <c r="G148" s="11"/>
+      <c r="H148" s="11"/>
+      <c r="I148" s="11"/>
+      <c r="J148" s="11"/>
+      <c r="K148" s="5"/>
+    </row>
+    <row r="149" spans="2:11">
+      <c r="B149" s="4"/>
+      <c r="C149" s="11"/>
+      <c r="D149" s="11"/>
+      <c r="E149" s="11"/>
+      <c r="F149" s="11"/>
+      <c r="G149" s="11"/>
+      <c r="H149" s="11"/>
+      <c r="I149" s="11"/>
+      <c r="J149" s="11"/>
+      <c r="K149" s="5"/>
+    </row>
+    <row r="150" spans="2:11">
+      <c r="B150" s="4"/>
+      <c r="C150" s="11"/>
+      <c r="D150" s="11"/>
+      <c r="E150" s="11"/>
+      <c r="F150" s="11"/>
+      <c r="G150" s="11"/>
+      <c r="H150" s="11"/>
+      <c r="I150" s="11"/>
+      <c r="J150" s="11"/>
+      <c r="K150" s="5"/>
+    </row>
+    <row r="151" spans="2:11">
+      <c r="B151" s="4"/>
+      <c r="C151" s="11"/>
+      <c r="D151" s="11"/>
+      <c r="E151" s="11"/>
+      <c r="F151" s="11"/>
+      <c r="G151" s="11"/>
+      <c r="H151" s="11"/>
+      <c r="I151" s="11"/>
+      <c r="J151" s="11"/>
+      <c r="K151" s="5"/>
+    </row>
+    <row r="152" spans="2:11">
+      <c r="B152" s="4"/>
+      <c r="C152" s="11"/>
+      <c r="D152" s="11"/>
+      <c r="E152" s="11"/>
+      <c r="F152" s="11"/>
+      <c r="G152" s="11"/>
+      <c r="H152" s="11"/>
+      <c r="I152" s="11"/>
+      <c r="J152" s="11"/>
+      <c r="K152" s="5"/>
+    </row>
+    <row r="153" spans="2:11">
+      <c r="B153" s="4"/>
+      <c r="C153" s="11"/>
+      <c r="D153" s="11"/>
+      <c r="E153" s="11"/>
+      <c r="F153" s="11"/>
+      <c r="G153" s="11"/>
+      <c r="H153" s="11"/>
+      <c r="I153" s="11"/>
+      <c r="J153" s="11"/>
+      <c r="K153" s="5"/>
+    </row>
+    <row r="154" spans="2:11">
+      <c r="B154" s="4"/>
+      <c r="C154" s="11"/>
+      <c r="D154" s="11"/>
+      <c r="E154" s="11"/>
+      <c r="F154" s="11"/>
+      <c r="G154" s="11"/>
+      <c r="H154" s="11"/>
+      <c r="I154" s="11"/>
+      <c r="J154" s="11"/>
+      <c r="K154" s="5"/>
+    </row>
+    <row r="155" spans="2:11">
+      <c r="B155" s="4"/>
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
+      <c r="E155" s="11"/>
+      <c r="F155" s="11"/>
+      <c r="G155" s="11"/>
+      <c r="H155" s="11"/>
+      <c r="I155" s="11"/>
+      <c r="J155" s="11"/>
+      <c r="K155" s="5"/>
+    </row>
+    <row r="156" spans="2:11">
+      <c r="B156" s="4"/>
+      <c r="C156" s="11"/>
+      <c r="D156" s="11"/>
+      <c r="E156" s="11"/>
+      <c r="F156" s="11"/>
+      <c r="G156" s="11"/>
+      <c r="H156" s="11"/>
+      <c r="I156" s="11"/>
+      <c r="J156" s="11"/>
+      <c r="K156" s="5"/>
+    </row>
+    <row r="157" spans="2:11">
+      <c r="B157" s="4"/>
+      <c r="C157" s="11"/>
+      <c r="D157" s="11"/>
+      <c r="E157" s="11"/>
+      <c r="F157" s="11"/>
+      <c r="G157" s="11"/>
+      <c r="H157" s="11"/>
+      <c r="I157" s="11"/>
+      <c r="J157" s="11"/>
+      <c r="K157" s="5"/>
+    </row>
+    <row r="158" spans="2:11">
+      <c r="B158" s="4"/>
+      <c r="C158" s="11"/>
+      <c r="D158" s="11"/>
+      <c r="E158" s="11"/>
+      <c r="F158" s="11"/>
+      <c r="G158" s="11"/>
+      <c r="H158" s="11"/>
+      <c r="I158" s="11"/>
+      <c r="J158" s="11"/>
+      <c r="K158" s="5"/>
+    </row>
+    <row r="159" spans="2:11">
+      <c r="B159" s="4"/>
+      <c r="C159" s="11"/>
+      <c r="D159" s="11"/>
+      <c r="E159" s="11"/>
+      <c r="F159" s="11"/>
+      <c r="G159" s="11"/>
+      <c r="H159" s="11"/>
+      <c r="I159" s="11"/>
+      <c r="J159" s="11"/>
+      <c r="K159" s="5"/>
+    </row>
+    <row r="160" spans="2:11">
+      <c r="B160" s="4"/>
+      <c r="C160" s="11"/>
+      <c r="D160" s="11"/>
+      <c r="E160" s="11"/>
+      <c r="F160" s="11"/>
+      <c r="G160" s="11"/>
+      <c r="H160" s="11"/>
+      <c r="I160" s="11"/>
+      <c r="J160" s="11"/>
+      <c r="K160" s="5"/>
+    </row>
+    <row r="161" spans="2:13">
+      <c r="B161" s="4"/>
+      <c r="C161" s="11"/>
+      <c r="D161" s="11"/>
+      <c r="E161" s="11"/>
+      <c r="F161" s="11"/>
+      <c r="G161" s="11"/>
+      <c r="H161" s="11"/>
+      <c r="I161" s="11"/>
+      <c r="J161" s="11"/>
+      <c r="K161" s="5"/>
+    </row>
+    <row r="162" spans="2:13">
+      <c r="B162" s="4"/>
+      <c r="C162" s="11"/>
+      <c r="D162" s="11"/>
+      <c r="E162" s="11"/>
+      <c r="F162" s="11"/>
+      <c r="G162" s="11"/>
+      <c r="H162" s="11"/>
+      <c r="I162" s="11"/>
+      <c r="J162" s="11"/>
+      <c r="K162" s="5"/>
+    </row>
+    <row r="163" spans="2:13">
+      <c r="B163" s="4"/>
+      <c r="C163" s="11"/>
+      <c r="D163" s="11"/>
+      <c r="E163" s="11"/>
+      <c r="F163" s="11"/>
+      <c r="G163" s="11"/>
+      <c r="H163" s="11"/>
+      <c r="I163" s="11"/>
+      <c r="J163" s="11"/>
+      <c r="K163" s="5"/>
+    </row>
+    <row r="164" spans="2:13">
+      <c r="B164" s="4"/>
+      <c r="C164" s="11"/>
+      <c r="D164" s="11"/>
+      <c r="E164" s="11"/>
+      <c r="F164" s="11"/>
+      <c r="G164" s="11"/>
+      <c r="H164" s="11"/>
+      <c r="I164" s="11"/>
+      <c r="J164" s="11"/>
+      <c r="K164" s="5"/>
+    </row>
+    <row r="165" spans="2:13">
+      <c r="B165" s="4"/>
+      <c r="C165" s="11"/>
+      <c r="D165" s="11"/>
+      <c r="E165" s="11"/>
+      <c r="F165" s="11"/>
+      <c r="G165" s="11"/>
+      <c r="H165" s="11"/>
+      <c r="I165" s="11"/>
+      <c r="J165" s="11"/>
+      <c r="K165" s="5"/>
+    </row>
+    <row r="166" spans="2:13">
+      <c r="B166" s="4"/>
+      <c r="C166" s="11"/>
+      <c r="D166" s="11"/>
+      <c r="E166" s="11"/>
+      <c r="F166" s="11"/>
+      <c r="G166" s="11"/>
+      <c r="H166" s="11"/>
+      <c r="I166" s="11"/>
+      <c r="J166" s="11"/>
+      <c r="K166" s="5"/>
+    </row>
+    <row r="167" spans="2:13">
+      <c r="B167" s="7"/>
+      <c r="C167" s="8"/>
+      <c r="D167" s="8"/>
+      <c r="E167" s="8"/>
+      <c r="F167" s="8"/>
+      <c r="G167" s="8"/>
+      <c r="H167" s="8"/>
+      <c r="I167" s="8"/>
+      <c r="J167" s="8"/>
+      <c r="K167" s="9"/>
+    </row>
+    <row r="170" spans="2:13">
+      <c r="B170" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="2"/>
+      <c r="H170" s="2"/>
+      <c r="I170" s="2"/>
+      <c r="J170" s="2"/>
+      <c r="K170" s="3"/>
+    </row>
+    <row r="171" spans="2:13">
+      <c r="B171" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C171" s="11"/>
+      <c r="D171" s="11"/>
+      <c r="E171" s="11"/>
+      <c r="F171" s="11"/>
+      <c r="G171" s="11"/>
+      <c r="H171" s="11"/>
+      <c r="I171" s="11"/>
+      <c r="J171" s="11"/>
+      <c r="K171" s="5"/>
+    </row>
+    <row r="172" spans="2:13">
+      <c r="B172" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C172" s="11"/>
+      <c r="D172" s="11"/>
+      <c r="E172" s="11"/>
+      <c r="F172" s="11"/>
+      <c r="G172" s="11"/>
+      <c r="H172" s="11"/>
+      <c r="I172" s="11"/>
+      <c r="J172" s="11"/>
+      <c r="K172" s="5"/>
+      <c r="L172" t="s">
+        <v>28</v>
+      </c>
+      <c r="M172" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="173" spans="2:13">
+      <c r="B173" s="4"/>
+      <c r="C173" s="11"/>
+      <c r="D173" s="11"/>
+      <c r="E173" s="11"/>
+      <c r="F173" s="11"/>
+      <c r="G173" s="11"/>
+      <c r="H173" s="11"/>
+      <c r="I173" s="11"/>
+      <c r="J173" s="11"/>
+      <c r="K173" s="5"/>
+      <c r="M173" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="174" spans="2:13">
+      <c r="B174" s="4"/>
+      <c r="C174" s="11"/>
+      <c r="D174" s="11"/>
+      <c r="E174" s="11"/>
+      <c r="F174" s="11"/>
+      <c r="G174" s="11"/>
+      <c r="H174" s="11"/>
+      <c r="I174" s="11"/>
+      <c r="J174" s="11"/>
+      <c r="K174" s="5"/>
+    </row>
+    <row r="175" spans="2:13">
+      <c r="B175" s="4"/>
+      <c r="C175" s="11"/>
+      <c r="D175" s="11"/>
+      <c r="E175" s="11"/>
+      <c r="F175" s="11"/>
+      <c r="G175" s="11"/>
+      <c r="H175" s="11"/>
+      <c r="I175" s="11"/>
+      <c r="J175" s="11"/>
+      <c r="K175" s="5"/>
+    </row>
+    <row r="176" spans="2:13">
+      <c r="B176" s="4"/>
+      <c r="C176" s="11"/>
+      <c r="D176" s="11"/>
+      <c r="E176" s="11"/>
+      <c r="F176" s="11"/>
+      <c r="G176" s="11"/>
+      <c r="H176" s="11"/>
+      <c r="I176" s="11"/>
+      <c r="J176" s="11"/>
+      <c r="K176" s="5"/>
+    </row>
+    <row r="177" spans="2:11">
+      <c r="B177" s="4"/>
+      <c r="C177" s="11"/>
+      <c r="D177" s="11"/>
+      <c r="E177" s="11"/>
+      <c r="F177" s="11"/>
+      <c r="G177" s="11"/>
+      <c r="H177" s="11"/>
+      <c r="I177" s="11"/>
+      <c r="J177" s="11"/>
+      <c r="K177" s="5"/>
+    </row>
+    <row r="178" spans="2:11">
+      <c r="B178" s="4"/>
+      <c r="C178" s="11"/>
+      <c r="D178" s="11"/>
+      <c r="E178" s="11"/>
+      <c r="F178" s="11"/>
+      <c r="G178" s="11"/>
+      <c r="H178" s="11"/>
+      <c r="I178" s="11"/>
+      <c r="J178" s="11"/>
+      <c r="K178" s="5"/>
+    </row>
+    <row r="179" spans="2:11">
+      <c r="B179" s="4"/>
+      <c r="C179" s="11"/>
+      <c r="D179" s="11"/>
+      <c r="E179" s="11"/>
+      <c r="F179" s="11"/>
+      <c r="G179" s="11"/>
+      <c r="H179" s="11"/>
+      <c r="I179" s="11"/>
+      <c r="J179" s="11"/>
+      <c r="K179" s="5"/>
+    </row>
+    <row r="180" spans="2:11">
+      <c r="B180" s="4"/>
+      <c r="C180" s="11"/>
+      <c r="D180" s="11"/>
+      <c r="E180" s="11"/>
+      <c r="F180" s="11"/>
+      <c r="G180" s="11"/>
+      <c r="H180" s="11"/>
+      <c r="I180" s="11"/>
+      <c r="J180" s="11"/>
+      <c r="K180" s="5"/>
+    </row>
+    <row r="181" spans="2:11">
+      <c r="B181" s="4"/>
+      <c r="C181" s="11"/>
+      <c r="D181" s="11"/>
+      <c r="E181" s="11"/>
+      <c r="F181" s="11"/>
+      <c r="G181" s="11"/>
+      <c r="H181" s="11"/>
+      <c r="I181" s="11"/>
+      <c r="J181" s="11"/>
+      <c r="K181" s="5"/>
+    </row>
+    <row r="182" spans="2:11">
+      <c r="B182" s="4"/>
+      <c r="C182" s="11"/>
+      <c r="D182" s="11"/>
+      <c r="E182" s="11"/>
+      <c r="F182" s="11"/>
+      <c r="G182" s="11"/>
+      <c r="H182" s="11"/>
+      <c r="I182" s="11"/>
+      <c r="J182" s="11"/>
+      <c r="K182" s="5"/>
+    </row>
+    <row r="183" spans="2:11">
+      <c r="B183" s="4"/>
+      <c r="C183" s="11"/>
+      <c r="D183" s="11"/>
+      <c r="E183" s="11"/>
+      <c r="F183" s="11"/>
+      <c r="G183" s="11"/>
+      <c r="H183" s="11"/>
+      <c r="I183" s="11"/>
+      <c r="J183" s="11"/>
+      <c r="K183" s="5"/>
+    </row>
+    <row r="184" spans="2:11">
+      <c r="B184" s="4"/>
+      <c r="C184" s="11"/>
+      <c r="D184" s="11"/>
+      <c r="E184" s="11"/>
+      <c r="F184" s="11"/>
+      <c r="G184" s="11"/>
+      <c r="H184" s="11"/>
+      <c r="I184" s="11"/>
+      <c r="J184" s="11"/>
+      <c r="K184" s="5"/>
+    </row>
+    <row r="185" spans="2:11">
+      <c r="B185" s="4"/>
+      <c r="C185" s="11"/>
+      <c r="D185" s="11"/>
+      <c r="E185" s="11"/>
+      <c r="F185" s="11"/>
+      <c r="G185" s="11"/>
+      <c r="H185" s="11"/>
+      <c r="I185" s="11"/>
+      <c r="J185" s="11"/>
+      <c r="K185" s="5"/>
+    </row>
+    <row r="186" spans="2:11">
+      <c r="B186" s="4"/>
+      <c r="C186" s="11"/>
+      <c r="D186" s="11"/>
+      <c r="E186" s="11"/>
+      <c r="F186" s="11"/>
+      <c r="G186" s="11"/>
+      <c r="H186" s="11"/>
+      <c r="I186" s="11"/>
+      <c r="J186" s="11"/>
+      <c r="K186" s="5"/>
+    </row>
+    <row r="187" spans="2:11">
+      <c r="B187" s="4"/>
+      <c r="C187" s="11"/>
+      <c r="D187" s="11"/>
+      <c r="E187" s="11"/>
+      <c r="F187" s="11"/>
+      <c r="G187" s="11"/>
+      <c r="H187" s="11"/>
+      <c r="I187" s="11"/>
+      <c r="J187" s="11"/>
+      <c r="K187" s="5"/>
+    </row>
+    <row r="188" spans="2:11">
+      <c r="B188" s="4"/>
+      <c r="C188" s="11"/>
+      <c r="D188" s="11"/>
+      <c r="E188" s="11"/>
+      <c r="F188" s="11"/>
+      <c r="G188" s="11"/>
+      <c r="H188" s="11"/>
+      <c r="I188" s="11"/>
+      <c r="J188" s="11"/>
+      <c r="K188" s="5"/>
+    </row>
+    <row r="189" spans="2:11">
+      <c r="B189" s="4"/>
+      <c r="C189" s="11"/>
+      <c r="D189" s="11"/>
+      <c r="E189" s="11"/>
+      <c r="F189" s="11"/>
+      <c r="G189" s="11"/>
+      <c r="H189" s="11"/>
+      <c r="I189" s="11"/>
+      <c r="J189" s="11"/>
+      <c r="K189" s="5"/>
+    </row>
+    <row r="190" spans="2:11">
+      <c r="B190" s="4"/>
+      <c r="C190" s="11"/>
+      <c r="D190" s="11"/>
+      <c r="E190" s="11"/>
+      <c r="F190" s="11"/>
+      <c r="G190" s="11"/>
+      <c r="H190" s="11"/>
+      <c r="I190" s="11"/>
+      <c r="J190" s="11"/>
+      <c r="K190" s="5"/>
+    </row>
+    <row r="191" spans="2:11">
+      <c r="B191" s="4"/>
+      <c r="C191" s="11"/>
+      <c r="D191" s="11"/>
+      <c r="E191" s="11"/>
+      <c r="F191" s="11"/>
+      <c r="G191" s="11"/>
+      <c r="H191" s="11"/>
+      <c r="I191" s="11"/>
+      <c r="J191" s="11"/>
+      <c r="K191" s="5"/>
+    </row>
+    <row r="192" spans="2:11">
+      <c r="B192" s="7"/>
+      <c r="C192" s="8"/>
+      <c r="D192" s="8"/>
+      <c r="E192" s="8"/>
+      <c r="F192" s="8"/>
+      <c r="G192" s="8"/>
+      <c r="H192" s="8"/>
+      <c r="I192" s="8"/>
+      <c r="J192" s="8"/>
+      <c r="K192" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>